<commit_message>
Added new schemes, docstrings, options for quadrant sampling and setting maximum tilt
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensities-Exp/AMstep1A.xlsx
+++ b/JupyterNotebooks/AveragedIntensities-Exp/AMstep1A.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>HKL</t>
   </si>
   <si>
     <t>Equal Angle</t>
+  </si>
+  <si>
+    <t>Bruker</t>
   </si>
   <si>
     <t>ND Single</t>
@@ -572,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -651,64 +654,64 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="U2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -719,64 +722,64 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8651666666666666</v>
+        <v>0.8702017291066283</v>
       </c>
       <c r="D3">
-        <v>0.9499444444444445</v>
+        <v>0.931664265129683</v>
       </c>
       <c r="E3">
-        <v>1.436805555555555</v>
+        <v>1.366131123919308</v>
       </c>
       <c r="F3">
-        <v>0.9689444444444445</v>
+        <v>0.9679971181556196</v>
       </c>
       <c r="G3">
-        <v>0.8651666666666666</v>
+        <v>0.8702017291066283</v>
       </c>
       <c r="H3">
-        <v>0.9499444444444445</v>
+        <v>0.931664265129683</v>
       </c>
       <c r="I3">
-        <v>0.9831388888888889</v>
+        <v>0.9938184438040346</v>
       </c>
       <c r="J3">
-        <v>1.105916666666667</v>
+        <v>1.095201729106628</v>
       </c>
       <c r="K3">
-        <v>0.8986666666666666</v>
+        <v>0.9067507204610951</v>
       </c>
       <c r="L3">
-        <v>0.9869166666666667</v>
+        <v>0.9789193083573487</v>
       </c>
       <c r="M3">
-        <v>0.8650833333333333</v>
+        <v>0.8701873198847262</v>
       </c>
       <c r="N3">
-        <v>0.8651666666666666</v>
+        <v>0.8702017291066283</v>
       </c>
       <c r="O3">
-        <v>1.193375</v>
+        <v>1.148897694524496</v>
       </c>
       <c r="P3">
-        <v>1.202875</v>
+        <v>1.167064121037464</v>
       </c>
       <c r="Q3">
-        <v>1.083972222222222</v>
+        <v>1.055999039385207</v>
       </c>
       <c r="R3">
-        <v>1.118564814814815</v>
+        <v>1.088597502401537</v>
       </c>
       <c r="S3">
-        <v>1.083972222222222</v>
+        <v>1.055999039385207</v>
       </c>
       <c r="T3">
-        <v>1.055215277777778</v>
+        <v>1.03399855907781</v>
       </c>
       <c r="U3">
-        <v>1.017205555555555</v>
+        <v>1.001239193083574</v>
       </c>
       <c r="V3">
-        <v>1.0244375</v>
+        <v>1.013835554755043</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -787,64 +790,64 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>1.01671778869646</v>
       </c>
       <c r="D4">
-        <v>0.33</v>
+        <v>1.034832282294812</v>
       </c>
       <c r="E4">
-        <v>4.81</v>
+        <v>0.9843386344991381</v>
       </c>
       <c r="F4">
-        <v>0.76</v>
+        <v>1.001257593302782</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>1.01671778869646</v>
       </c>
       <c r="H4">
-        <v>0.33</v>
+        <v>1.034832282294812</v>
       </c>
       <c r="I4">
-        <v>0.73</v>
+        <v>0.9855685745116541</v>
       </c>
       <c r="J4">
-        <v>2.02</v>
+        <v>0.97749173078137</v>
       </c>
       <c r="K4">
-        <v>0.25</v>
+        <v>1.001171305701348</v>
       </c>
       <c r="L4">
-        <v>0.92</v>
+        <v>1.00258831739364</v>
       </c>
       <c r="M4">
-        <v>0.1</v>
+        <v>1.016697852763461</v>
       </c>
       <c r="N4">
-        <v>0.1</v>
+        <v>1.01671778869646</v>
       </c>
       <c r="O4">
-        <v>2.57</v>
+        <v>1.009585458396975</v>
       </c>
       <c r="P4">
-        <v>2.785</v>
+        <v>0.99279811390096</v>
       </c>
       <c r="Q4">
-        <v>1.746666666666666</v>
+        <v>1.011962901830137</v>
       </c>
       <c r="R4">
-        <v>1.966666666666667</v>
+        <v>1.006809503365577</v>
       </c>
       <c r="S4">
-        <v>1.746666666666666</v>
+        <v>1.011962901830136</v>
       </c>
       <c r="T4">
-        <v>1.5</v>
+        <v>1.009286574698298</v>
       </c>
       <c r="U4">
-        <v>1.22</v>
+        <v>1.01077281749793</v>
       </c>
       <c r="V4">
-        <v>1.24</v>
+        <v>1.00049577839765</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -855,64 +858,64 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1.18</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
-        <v>2.06</v>
+        <v>0.33</v>
       </c>
       <c r="E5">
-        <v>0.59</v>
+        <v>4.81</v>
       </c>
       <c r="F5">
-        <v>1.25</v>
+        <v>0.76</v>
       </c>
       <c r="G5">
-        <v>1.18</v>
+        <v>0.1</v>
       </c>
       <c r="H5">
-        <v>2.06</v>
+        <v>0.33</v>
       </c>
       <c r="I5">
-        <v>0.85</v>
+        <v>0.73</v>
       </c>
       <c r="J5">
-        <v>0.49</v>
+        <v>2.02</v>
       </c>
       <c r="K5">
-        <v>1.2</v>
+        <v>0.25</v>
       </c>
       <c r="L5">
-        <v>1.53</v>
+        <v>0.92</v>
       </c>
       <c r="M5">
-        <v>1.18</v>
+        <v>0.1</v>
       </c>
       <c r="N5">
-        <v>1.18</v>
+        <v>0.1</v>
       </c>
       <c r="O5">
-        <v>1.325</v>
+        <v>2.57</v>
       </c>
       <c r="P5">
-        <v>0.9199999999999999</v>
+        <v>2.785</v>
       </c>
       <c r="Q5">
-        <v>1.276666666666667</v>
+        <v>1.746666666666666</v>
       </c>
       <c r="R5">
-        <v>1.3</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="S5">
-        <v>1.276666666666667</v>
+        <v>1.746666666666666</v>
       </c>
       <c r="T5">
-        <v>1.27</v>
+        <v>1.5</v>
       </c>
       <c r="U5">
-        <v>1.252</v>
+        <v>1.22</v>
       </c>
       <c r="V5">
-        <v>1.14375</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -923,64 +926,64 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1.16</v>
+        <v>1.18</v>
       </c>
       <c r="D6">
-        <v>1.14</v>
+        <v>2.06</v>
       </c>
       <c r="E6">
-        <v>0.67</v>
+        <v>0.59</v>
       </c>
       <c r="F6">
-        <v>1.19</v>
+        <v>1.25</v>
       </c>
       <c r="G6">
-        <v>1.16</v>
+        <v>1.18</v>
       </c>
       <c r="H6">
-        <v>1.14</v>
+        <v>2.06</v>
       </c>
       <c r="I6">
-        <v>1.03</v>
+        <v>0.85</v>
       </c>
       <c r="J6">
-        <v>0.6</v>
+        <v>0.49</v>
       </c>
       <c r="K6">
+        <v>1.2</v>
+      </c>
+      <c r="L6">
+        <v>1.53</v>
+      </c>
+      <c r="M6">
         <v>1.18</v>
       </c>
-      <c r="L6">
-        <v>1.2</v>
-      </c>
-      <c r="M6">
-        <v>1.16</v>
-      </c>
       <c r="N6">
-        <v>1.16</v>
+        <v>1.18</v>
       </c>
       <c r="O6">
-        <v>0.905</v>
+        <v>1.325</v>
       </c>
       <c r="P6">
-        <v>0.9299999999999999</v>
+        <v>0.9199999999999999</v>
       </c>
       <c r="Q6">
-        <v>0.9899999999999999</v>
+        <v>1.276666666666667</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="S6">
-        <v>0.9899999999999999</v>
+        <v>1.276666666666667</v>
       </c>
       <c r="T6">
-        <v>1.04</v>
+        <v>1.27</v>
       </c>
       <c r="U6">
-        <v>1.064</v>
+        <v>1.252</v>
       </c>
       <c r="V6">
-        <v>1.02125</v>
+        <v>1.14375</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -991,64 +994,64 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.44</v>
+        <v>1.16</v>
       </c>
       <c r="D7">
-        <v>0.68</v>
+        <v>1.14</v>
       </c>
       <c r="E7">
-        <v>1.67</v>
+        <v>0.67</v>
       </c>
       <c r="F7">
+        <v>1.19</v>
+      </c>
+      <c r="G7">
         <v>1.16</v>
       </c>
-      <c r="G7">
-        <v>0.44</v>
-      </c>
       <c r="H7">
-        <v>0.68</v>
+        <v>1.14</v>
       </c>
       <c r="I7">
-        <v>0.99</v>
+        <v>1.03</v>
       </c>
       <c r="J7">
-        <v>1.06</v>
+        <v>0.6</v>
       </c>
       <c r="K7">
-        <v>0.85</v>
+        <v>1.18</v>
       </c>
       <c r="L7">
-        <v>0.97</v>
+        <v>1.2</v>
       </c>
       <c r="M7">
-        <v>0.44</v>
+        <v>1.16</v>
       </c>
       <c r="N7">
-        <v>0.44</v>
+        <v>1.16</v>
       </c>
       <c r="O7">
-        <v>1.175</v>
+        <v>0.905</v>
       </c>
       <c r="P7">
-        <v>1.415</v>
+        <v>0.9299999999999999</v>
       </c>
       <c r="Q7">
-        <v>0.93</v>
+        <v>0.9899999999999999</v>
       </c>
       <c r="R7">
-        <v>1.17</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>0.93</v>
+        <v>0.9899999999999999</v>
       </c>
       <c r="T7">
-        <v>0.9875</v>
+        <v>1.04</v>
       </c>
       <c r="U7">
-        <v>0.8780000000000001</v>
+        <v>1.064</v>
       </c>
       <c r="V7">
-        <v>0.9775</v>
+        <v>1.02125</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1059,64 +1062,64 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1.527534246575343</v>
+        <v>0.44</v>
       </c>
       <c r="D8">
-        <v>1.986986301369863</v>
+        <v>0.68</v>
       </c>
       <c r="E8">
-        <v>0.6938356164383561</v>
+        <v>1.67</v>
       </c>
       <c r="F8">
-        <v>1.206986301369863</v>
+        <v>1.16</v>
       </c>
       <c r="G8">
-        <v>1.527534246575343</v>
+        <v>0.44</v>
       </c>
       <c r="H8">
-        <v>1.986986301369863</v>
+        <v>0.68</v>
       </c>
       <c r="I8">
-        <v>0.8423287671232876</v>
+        <v>0.99</v>
       </c>
       <c r="J8">
-        <v>0.586986301369863</v>
+        <v>1.06</v>
       </c>
       <c r="K8">
-        <v>1.221506849315068</v>
+        <v>0.85</v>
       </c>
       <c r="L8">
-        <v>1.272739726027397</v>
+        <v>0.97</v>
       </c>
       <c r="M8">
-        <v>1.526575342465753</v>
+        <v>0.44</v>
       </c>
       <c r="N8">
-        <v>1.527534246575343</v>
+        <v>0.44</v>
       </c>
       <c r="O8">
-        <v>1.34041095890411</v>
+        <v>1.175</v>
       </c>
       <c r="P8">
-        <v>0.9504109589041095</v>
+        <v>1.415</v>
       </c>
       <c r="Q8">
-        <v>1.402785388127854</v>
+        <v>0.93</v>
       </c>
       <c r="R8">
-        <v>1.295936073059361</v>
+        <v>1.17</v>
       </c>
       <c r="S8">
-        <v>1.402785388127854</v>
+        <v>0.93</v>
       </c>
       <c r="T8">
-        <v>1.353835616438356</v>
+        <v>0.9875</v>
       </c>
       <c r="U8">
-        <v>1.388575342465753</v>
+        <v>0.8780000000000001</v>
       </c>
       <c r="V8">
-        <v>1.16736301369863</v>
+        <v>0.9775</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1127,64 +1130,64 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.8394736842105263</v>
+        <v>1.527534246575343</v>
       </c>
       <c r="D9">
-        <v>0.9010526315789473</v>
+        <v>1.986986301369863</v>
       </c>
       <c r="E9">
-        <v>1.426842105263158</v>
+        <v>0.6938356164383561</v>
       </c>
       <c r="F9">
-        <v>0.9336842105263158</v>
+        <v>1.206986301369863</v>
       </c>
       <c r="G9">
-        <v>0.8394736842105263</v>
+        <v>1.527534246575343</v>
       </c>
       <c r="H9">
-        <v>0.9010526315789473</v>
+        <v>1.986986301369863</v>
       </c>
       <c r="I9">
-        <v>0.9947368421052631</v>
+        <v>0.8423287671232876</v>
       </c>
       <c r="J9">
-        <v>1.13</v>
+        <v>0.586986301369863</v>
       </c>
       <c r="K9">
-        <v>0.8436842105263158</v>
+        <v>1.221506849315068</v>
       </c>
       <c r="L9">
-        <v>1.027894736842105</v>
+        <v>1.272739726027397</v>
       </c>
       <c r="M9">
-        <v>0.8389473684210527</v>
+        <v>1.526575342465753</v>
       </c>
       <c r="N9">
-        <v>0.8394736842105263</v>
+        <v>1.527534246575343</v>
       </c>
       <c r="O9">
-        <v>1.163947368421053</v>
+        <v>1.34041095890411</v>
       </c>
       <c r="P9">
-        <v>1.180263157894737</v>
+        <v>0.9504109589041095</v>
       </c>
       <c r="Q9">
-        <v>1.055789473684211</v>
+        <v>1.402785388127854</v>
       </c>
       <c r="R9">
-        <v>1.08719298245614</v>
+        <v>1.295936073059361</v>
       </c>
       <c r="S9">
-        <v>1.055789473684211</v>
+        <v>1.402785388127854</v>
       </c>
       <c r="T9">
-        <v>1.025263157894737</v>
+        <v>1.353835616438356</v>
       </c>
       <c r="U9">
-        <v>0.9881052631578948</v>
+        <v>1.388575342465753</v>
       </c>
       <c r="V9">
-        <v>1.012171052631579</v>
+        <v>1.16736301369863</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1195,64 +1198,64 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.9478947368421052</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="D10">
-        <v>0.838421052631579</v>
+        <v>0.9010526315789473</v>
       </c>
       <c r="E10">
-        <v>1.286315789473684</v>
+        <v>1.426842105263158</v>
       </c>
       <c r="F10">
-        <v>0.9821052631578947</v>
+        <v>0.9336842105263158</v>
       </c>
       <c r="G10">
-        <v>0.9478947368421052</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="H10">
-        <v>0.838421052631579</v>
+        <v>0.9010526315789473</v>
       </c>
       <c r="I10">
-        <v>1.016842105263158</v>
+        <v>0.9947368421052631</v>
       </c>
       <c r="J10">
-        <v>1.057368421052632</v>
+        <v>1.13</v>
       </c>
       <c r="K10">
-        <v>0.9178947368421052</v>
+        <v>0.8436842105263158</v>
       </c>
       <c r="L10">
-        <v>0.9694736842105263</v>
+        <v>1.027894736842105</v>
       </c>
       <c r="M10">
-        <v>0.9484210526315789</v>
+        <v>0.8389473684210527</v>
       </c>
       <c r="N10">
-        <v>0.9478947368421052</v>
+        <v>0.8394736842105263</v>
       </c>
       <c r="O10">
-        <v>1.062368421052632</v>
+        <v>1.163947368421053</v>
       </c>
       <c r="P10">
-        <v>1.13421052631579</v>
+        <v>1.180263157894737</v>
       </c>
       <c r="Q10">
-        <v>1.024210526315789</v>
+        <v>1.055789473684211</v>
       </c>
       <c r="R10">
-        <v>1.035614035087719</v>
+        <v>1.08719298245614</v>
       </c>
       <c r="S10">
-        <v>1.024210526315789</v>
+        <v>1.055789473684211</v>
       </c>
       <c r="T10">
-        <v>1.013684210526316</v>
+        <v>1.025263157894737</v>
       </c>
       <c r="U10">
-        <v>1.000526315789474</v>
+        <v>0.9881052631578948</v>
       </c>
       <c r="V10">
-        <v>1.002039473684211</v>
+        <v>1.012171052631579</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1263,64 +1266,64 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.4897480000000001</v>
+        <v>0.9478947368421052</v>
       </c>
       <c r="D11">
-        <v>0.5474439999999994</v>
+        <v>0.838421052631579</v>
       </c>
       <c r="E11">
-        <v>3.091227999999997</v>
+        <v>1.286315789473684</v>
       </c>
       <c r="F11">
-        <v>0.8549679999999996</v>
+        <v>0.9821052631578947</v>
       </c>
       <c r="G11">
-        <v>0.4897480000000001</v>
+        <v>0.9478947368421052</v>
       </c>
       <c r="H11">
-        <v>0.5474439999999994</v>
+        <v>0.838421052631579</v>
       </c>
       <c r="I11">
-        <v>0.9067239999999994</v>
+        <v>1.016842105263158</v>
       </c>
       <c r="J11">
-        <v>1.536004</v>
+        <v>1.057368421052632</v>
       </c>
       <c r="K11">
-        <v>0.579956</v>
+        <v>0.9178947368421052</v>
       </c>
       <c r="L11">
-        <v>0.9322440000000021</v>
+        <v>0.9694736842105263</v>
       </c>
       <c r="M11">
-        <v>0.4897480000000001</v>
+        <v>0.9484210526315789</v>
       </c>
       <c r="N11">
-        <v>0.4897480000000001</v>
+        <v>0.9478947368421052</v>
       </c>
       <c r="O11">
-        <v>1.819335999999999</v>
+        <v>1.062368421052632</v>
       </c>
       <c r="P11">
-        <v>1.973097999999998</v>
+        <v>1.13421052631579</v>
       </c>
       <c r="Q11">
-        <v>1.376139999999999</v>
+        <v>1.024210526315789</v>
       </c>
       <c r="R11">
-        <v>1.497879999999999</v>
+        <v>1.035614035087719</v>
       </c>
       <c r="S11">
-        <v>1.376139999999999</v>
+        <v>1.024210526315789</v>
       </c>
       <c r="T11">
-        <v>1.245846999999999</v>
+        <v>1.013684210526316</v>
       </c>
       <c r="U11">
-        <v>1.094627199999999</v>
+        <v>1.000526315789474</v>
       </c>
       <c r="V11">
-        <v>1.1172895</v>
+        <v>1.002039473684211</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -1331,64 +1334,64 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.4897480000000001</v>
       </c>
       <c r="D12">
-        <v>0.33</v>
+        <v>0.5474439999999994</v>
       </c>
       <c r="E12">
-        <v>4.813462499999997</v>
+        <v>3.091227999999997</v>
       </c>
       <c r="F12">
-        <v>0.76</v>
+        <v>0.8549679999999996</v>
       </c>
       <c r="G12">
-        <v>0.1</v>
+        <v>0.4897480000000001</v>
       </c>
       <c r="H12">
-        <v>0.33</v>
+        <v>0.5474439999999994</v>
       </c>
       <c r="I12">
-        <v>0.73</v>
+        <v>0.9067239999999994</v>
       </c>
       <c r="J12">
-        <v>2.014012499999999</v>
+        <v>1.536004</v>
       </c>
       <c r="K12">
-        <v>0.25</v>
+        <v>0.579956</v>
       </c>
       <c r="L12">
-        <v>0.92</v>
+        <v>0.9322440000000021</v>
       </c>
       <c r="M12">
-        <v>0.1</v>
+        <v>0.4897480000000001</v>
       </c>
       <c r="N12">
-        <v>0.1</v>
+        <v>0.4897480000000001</v>
       </c>
       <c r="O12">
-        <v>2.571731249999999</v>
+        <v>1.819335999999999</v>
       </c>
       <c r="P12">
-        <v>2.786731249999999</v>
+        <v>1.973097999999998</v>
       </c>
       <c r="Q12">
-        <v>1.747820833333332</v>
+        <v>1.376139999999999</v>
       </c>
       <c r="R12">
-        <v>1.967820833333332</v>
+        <v>1.497879999999999</v>
       </c>
       <c r="S12">
-        <v>1.747820833333332</v>
+        <v>1.376139999999999</v>
       </c>
       <c r="T12">
-        <v>1.500865624999999</v>
+        <v>1.245846999999999</v>
       </c>
       <c r="U12">
-        <v>1.220692499999999</v>
+        <v>1.094627199999999</v>
       </c>
       <c r="V12">
-        <v>1.239684375</v>
+        <v>1.1172895</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1399,64 +1402,64 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.4674621114368007</v>
+        <v>0.1</v>
       </c>
       <c r="D13">
-        <v>0.6192970245120014</v>
+        <v>0.33</v>
       </c>
       <c r="E13">
-        <v>3.119397813759996</v>
+        <v>4.813462499999997</v>
       </c>
       <c r="F13">
-        <v>0.8510115180543998</v>
+        <v>0.76</v>
       </c>
       <c r="G13">
-        <v>0.4674621114368007</v>
+        <v>0.1</v>
       </c>
       <c r="H13">
-        <v>0.6192970245120014</v>
+        <v>0.33</v>
       </c>
       <c r="I13">
-        <v>0.8743443001344013</v>
+        <v>0.73</v>
       </c>
       <c r="J13">
-        <v>1.559972120473593</v>
+        <v>2.014012499999999</v>
       </c>
       <c r="K13">
-        <v>0.5694234562560009</v>
+        <v>0.25</v>
       </c>
       <c r="L13">
-        <v>0.9422501428223996</v>
+        <v>0.92</v>
       </c>
       <c r="M13">
-        <v>0.4674975526912008</v>
+        <v>0.1</v>
       </c>
       <c r="N13">
-        <v>0.4674621114368007</v>
+        <v>0.1</v>
       </c>
       <c r="O13">
-        <v>1.869347419135999</v>
+        <v>2.571731249999999</v>
       </c>
       <c r="P13">
-        <v>1.985204665907198</v>
+        <v>2.786731249999999</v>
       </c>
       <c r="Q13">
-        <v>1.402052316569599</v>
+        <v>1.747820833333332</v>
       </c>
       <c r="R13">
-        <v>1.529902118775466</v>
+        <v>1.967820833333332</v>
       </c>
       <c r="S13">
-        <v>1.402052316569599</v>
+        <v>1.747820833333332</v>
       </c>
       <c r="T13">
-        <v>1.2642921169408</v>
+        <v>1.500865624999999</v>
       </c>
       <c r="U13">
-        <v>1.10492611584</v>
+        <v>1.220692499999999</v>
       </c>
       <c r="V13">
-        <v>1.125394810931199</v>
+        <v>1.239684375</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1467,64 +1470,64 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0.996367802053426</v>
+        <v>0.4674621114368007</v>
       </c>
       <c r="D14">
-        <v>0.995457787320688</v>
+        <v>0.6192970245120014</v>
       </c>
       <c r="E14">
-        <v>0.9999552083363917</v>
+        <v>3.119397813759996</v>
       </c>
       <c r="F14">
-        <v>0.9921241659138282</v>
+        <v>0.8510115180543998</v>
       </c>
       <c r="G14">
-        <v>0.996367802053426</v>
+        <v>0.4674621114368007</v>
       </c>
       <c r="H14">
-        <v>0.995457787320688</v>
+        <v>0.6192970245120014</v>
       </c>
       <c r="I14">
-        <v>0.9906768381245873</v>
+        <v>0.8743443001344013</v>
       </c>
       <c r="J14">
-        <v>0.994522282028472</v>
+        <v>1.559972120473593</v>
       </c>
       <c r="K14">
-        <v>0.991456004279841</v>
+        <v>0.5694234562560009</v>
       </c>
       <c r="L14">
-        <v>0.9909658137760419</v>
+        <v>0.9422501428223996</v>
       </c>
       <c r="M14">
-        <v>0.9963722216287327</v>
+        <v>0.4674975526912008</v>
       </c>
       <c r="N14">
-        <v>0.996367802053426</v>
+        <v>0.4674621114368007</v>
       </c>
       <c r="O14">
-        <v>0.9977064978285399</v>
+        <v>1.869347419135999</v>
       </c>
       <c r="P14">
-        <v>0.99603968712511</v>
+        <v>1.985204665907198</v>
       </c>
       <c r="Q14">
-        <v>0.997260265903502</v>
+        <v>1.402052316569599</v>
       </c>
       <c r="R14">
-        <v>0.9958457205236361</v>
+        <v>1.529902118775466</v>
       </c>
       <c r="S14">
-        <v>0.9972602659035018</v>
+        <v>1.402052316569599</v>
       </c>
       <c r="T14">
-        <v>0.9959762409060835</v>
+        <v>1.2642921169408</v>
       </c>
       <c r="U14">
-        <v>0.9960545531355519</v>
+        <v>1.10492611584</v>
       </c>
       <c r="V14">
-        <v>0.9939407377291596</v>
+        <v>1.125394810931199</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -1535,64 +1538,64 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>1.024710639967963</v>
+        <v>0.996367802053426</v>
       </c>
       <c r="D15">
-        <v>1.030837120684621</v>
+        <v>0.995457787320688</v>
       </c>
       <c r="E15">
-        <v>1.003746833203462</v>
+        <v>0.9999552083363917</v>
       </c>
       <c r="F15">
-        <v>0.9683346361025379</v>
+        <v>0.9921241659138282</v>
       </c>
       <c r="G15">
-        <v>1.024710639967963</v>
+        <v>0.996367802053426</v>
       </c>
       <c r="H15">
-        <v>1.030837120684621</v>
+        <v>0.995457787320688</v>
       </c>
       <c r="I15">
-        <v>1.006991845687499</v>
+        <v>0.9906768381245873</v>
       </c>
       <c r="J15">
-        <v>0.9576019447326357</v>
+        <v>0.994522282028472</v>
       </c>
       <c r="K15">
-        <v>1.005600969736321</v>
+        <v>0.991456004279841</v>
       </c>
       <c r="L15">
-        <v>0.9906942000317984</v>
+        <v>0.9909658137760419</v>
       </c>
       <c r="M15">
-        <v>1.024800319465982</v>
+        <v>0.9963722216287327</v>
       </c>
       <c r="N15">
-        <v>1.024710639967963</v>
+        <v>0.996367802053426</v>
       </c>
       <c r="O15">
-        <v>1.017291976944041</v>
+        <v>0.9977064978285399</v>
       </c>
       <c r="P15">
-        <v>0.986040734653</v>
+        <v>0.99603968712511</v>
       </c>
       <c r="Q15">
-        <v>1.019764864618682</v>
+        <v>0.997260265903502</v>
       </c>
       <c r="R15">
-        <v>1.000972863330207</v>
+        <v>0.9958457205236361</v>
       </c>
       <c r="S15">
-        <v>1.019764864618682</v>
+        <v>0.9972602659035018</v>
       </c>
       <c r="T15">
-        <v>1.006907307489646</v>
+        <v>0.9959762409060835</v>
       </c>
       <c r="U15">
-        <v>1.010467973985309</v>
+        <v>0.9960545531355519</v>
       </c>
       <c r="V15">
-        <v>0.9985647737683547</v>
+        <v>0.9939407377291596</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1603,64 +1606,64 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>1.127203406092757</v>
+        <v>1.024710639967963</v>
       </c>
       <c r="D16">
-        <v>1.098311226622441</v>
+        <v>1.030837120684621</v>
       </c>
       <c r="E16">
-        <v>0.849701164557307</v>
+        <v>1.003746833203462</v>
       </c>
       <c r="F16">
-        <v>0.954676772895073</v>
+        <v>0.9683346361025379</v>
       </c>
       <c r="G16">
-        <v>1.127203406092757</v>
+        <v>1.024710639967963</v>
       </c>
       <c r="H16">
-        <v>1.098311226622441</v>
+        <v>1.030837120684621</v>
       </c>
       <c r="I16">
-        <v>0.9400886750822883</v>
+        <v>1.006991845687499</v>
       </c>
       <c r="J16">
-        <v>0.9851332635722462</v>
+        <v>0.9576019447326357</v>
       </c>
       <c r="K16">
-        <v>0.9574205927008589</v>
+        <v>1.005600969736321</v>
       </c>
       <c r="L16">
-        <v>1.038633751827486</v>
+        <v>0.9906942000317984</v>
       </c>
       <c r="M16">
-        <v>1.128389164784767</v>
+        <v>1.024800319465982</v>
       </c>
       <c r="N16">
-        <v>1.127203406092757</v>
+        <v>1.024710639967963</v>
       </c>
       <c r="O16">
-        <v>0.9740061955898738</v>
+        <v>1.017291976944041</v>
       </c>
       <c r="P16">
-        <v>0.90218896872619</v>
+        <v>0.986040734653</v>
       </c>
       <c r="Q16">
-        <v>1.025071932424168</v>
+        <v>1.019764864618682</v>
       </c>
       <c r="R16">
-        <v>0.9675630546916069</v>
+        <v>1.000972863330207</v>
       </c>
       <c r="S16">
-        <v>1.025071932424168</v>
+        <v>1.019764864618682</v>
       </c>
       <c r="T16">
-        <v>1.007473142541894</v>
+        <v>1.006907307489646</v>
       </c>
       <c r="U16">
-        <v>1.031419195252067</v>
+        <v>1.010467973985309</v>
       </c>
       <c r="V16">
-        <v>0.993896106668807</v>
+        <v>0.9985647737683547</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -1671,64 +1674,64 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>0.9600251887230775</v>
+        <v>1.127203406092757</v>
       </c>
       <c r="D17">
-        <v>0.9865505020058352</v>
+        <v>1.098311226622441</v>
       </c>
       <c r="E17">
-        <v>1.019340319888624</v>
+        <v>0.849701164557307</v>
       </c>
       <c r="F17">
-        <v>0.9920949529131629</v>
+        <v>0.954676772895073</v>
       </c>
       <c r="G17">
-        <v>0.9600251887230775</v>
+        <v>1.127203406092757</v>
       </c>
       <c r="H17">
-        <v>0.9865505020058352</v>
+        <v>1.098311226622441</v>
       </c>
       <c r="I17">
-        <v>0.9947958050906347</v>
+        <v>0.9400886750822883</v>
       </c>
       <c r="J17">
-        <v>1.005524929935368</v>
+        <v>0.9851332635722462</v>
       </c>
       <c r="K17">
-        <v>0.9789180482180128</v>
+        <v>0.9574205927008589</v>
       </c>
       <c r="L17">
-        <v>0.9958690063428771</v>
+        <v>1.038633751827486</v>
       </c>
       <c r="M17">
-        <v>0.9600319254103579</v>
+        <v>1.128389164784767</v>
       </c>
       <c r="N17">
-        <v>0.9600251887230775</v>
+        <v>1.127203406092757</v>
       </c>
       <c r="O17">
-        <v>1.00294541094723</v>
+        <v>0.9740061955898738</v>
       </c>
       <c r="P17">
-        <v>1.005717636400894</v>
+        <v>0.90218896872619</v>
       </c>
       <c r="Q17">
-        <v>0.9886386702058455</v>
+        <v>1.025071932424168</v>
       </c>
       <c r="R17">
-        <v>0.9993285916025406</v>
+        <v>0.9675630546916069</v>
       </c>
       <c r="S17">
-        <v>0.9886386702058457</v>
+        <v>1.025071932424168</v>
       </c>
       <c r="T17">
-        <v>0.989502740882675</v>
+        <v>1.007473142541894</v>
       </c>
       <c r="U17">
-        <v>0.9836072304507555</v>
+        <v>1.031419195252067</v>
       </c>
       <c r="V17">
-        <v>0.991639844139699</v>
+        <v>0.993896106668807</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -1739,64 +1742,64 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>0.9797488190998223</v>
+        <v>0.9600251887230775</v>
       </c>
       <c r="D18">
-        <v>1.015294969040166</v>
+        <v>0.9865505020058352</v>
       </c>
       <c r="E18">
-        <v>0.9483105311152336</v>
+        <v>1.019340319888624</v>
       </c>
       <c r="F18">
-        <v>1.004771369321141</v>
+        <v>0.9920949529131629</v>
       </c>
       <c r="G18">
-        <v>0.9797488190998223</v>
+        <v>0.9600251887230775</v>
       </c>
       <c r="H18">
-        <v>1.015294969040166</v>
+        <v>0.9865505020058352</v>
       </c>
       <c r="I18">
-        <v>1.000407181346143</v>
+        <v>0.9947958050906347</v>
       </c>
       <c r="J18">
-        <v>0.9823508500147028</v>
+        <v>1.005524929935368</v>
       </c>
       <c r="K18">
-        <v>0.9976520600810181</v>
+        <v>0.9789180482180128</v>
       </c>
       <c r="L18">
-        <v>1.007410485335057</v>
+        <v>0.9958690063428771</v>
       </c>
       <c r="M18">
-        <v>0.980156308306807</v>
+        <v>0.9600319254103579</v>
       </c>
       <c r="N18">
-        <v>0.9797488190998223</v>
+        <v>0.9600251887230775</v>
       </c>
       <c r="O18">
-        <v>0.9818027500776996</v>
+        <v>1.00294541094723</v>
       </c>
       <c r="P18">
-        <v>0.9765409502181871</v>
+        <v>1.005717636400894</v>
       </c>
       <c r="Q18">
-        <v>0.9811181064184072</v>
+        <v>0.9886386702058455</v>
       </c>
       <c r="R18">
-        <v>0.98945895649218</v>
+        <v>0.9993285916025406</v>
       </c>
       <c r="S18">
-        <v>0.9811181064184072</v>
+        <v>0.9886386702058457</v>
       </c>
       <c r="T18">
-        <v>0.9870314221440906</v>
+        <v>0.989502740882675</v>
       </c>
       <c r="U18">
-        <v>0.985574901535237</v>
+        <v>0.9836072304507555</v>
       </c>
       <c r="V18">
-        <v>0.9919932831691602</v>
+        <v>0.991639844139699</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -1807,64 +1810,64 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>1.013006910173542</v>
+        <v>0.9797488190998223</v>
       </c>
       <c r="D19">
-        <v>0.9873769606520982</v>
+        <v>1.015294969040166</v>
       </c>
       <c r="E19">
-        <v>0.9405576759389568</v>
+        <v>0.9483105311152336</v>
       </c>
       <c r="F19">
-        <v>1.033481381736685</v>
+        <v>1.004771369321141</v>
       </c>
       <c r="G19">
-        <v>1.013006910173542</v>
+        <v>0.9797488190998223</v>
       </c>
       <c r="H19">
-        <v>0.9873769606520982</v>
+        <v>1.015294969040166</v>
       </c>
       <c r="I19">
-        <v>0.9670113740018323</v>
+        <v>1.000407181346143</v>
       </c>
       <c r="J19">
-        <v>0.9891447521153021</v>
+        <v>0.9823508500147028</v>
       </c>
       <c r="K19">
-        <v>0.9629808154079396</v>
+        <v>0.9976520600810181</v>
       </c>
       <c r="L19">
-        <v>1.018247245402604</v>
+        <v>1.007410485335057</v>
       </c>
       <c r="M19">
-        <v>1.014052326014955</v>
+        <v>0.980156308306807</v>
       </c>
       <c r="N19">
-        <v>1.013006910173542</v>
+        <v>0.9797488190998223</v>
       </c>
       <c r="O19">
-        <v>0.9639673182955275</v>
+        <v>0.9818027500776996</v>
       </c>
       <c r="P19">
-        <v>0.9870195288378207</v>
+        <v>0.9765409502181871</v>
       </c>
       <c r="Q19">
-        <v>0.9803138489215323</v>
+        <v>0.9811181064184072</v>
       </c>
       <c r="R19">
-        <v>0.9871386727759132</v>
+        <v>0.98945895649218</v>
       </c>
       <c r="S19">
-        <v>0.9803138489215324</v>
+        <v>0.9811181064184072</v>
       </c>
       <c r="T19">
-        <v>0.9936057321253204</v>
+        <v>0.9870314221440906</v>
       </c>
       <c r="U19">
-        <v>0.9974859677349647</v>
+        <v>0.985574901535237</v>
       </c>
       <c r="V19">
-        <v>0.98897588942862</v>
+        <v>0.9919932831691602</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -1875,64 +1878,64 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>1.0661482908144</v>
+        <v>1.013006910173542</v>
       </c>
       <c r="D20">
-        <v>1.157420624855248</v>
+        <v>0.9873769606520982</v>
       </c>
       <c r="E20">
-        <v>0.9532387619054798</v>
+        <v>0.9405576759389568</v>
       </c>
       <c r="F20">
-        <v>1.119458973158533</v>
+        <v>1.033481381736685</v>
       </c>
       <c r="G20">
-        <v>1.0661482908144</v>
+        <v>1.013006910173542</v>
       </c>
       <c r="H20">
-        <v>1.157420624855248</v>
+        <v>0.9873769606520982</v>
       </c>
       <c r="I20">
-        <v>0.9258962165137228</v>
+        <v>0.9670113740018323</v>
       </c>
       <c r="J20">
-        <v>0.8128883259974095</v>
+        <v>0.9891447521153021</v>
       </c>
       <c r="K20">
-        <v>1.139780502081307</v>
+        <v>0.9629808154079396</v>
       </c>
       <c r="L20">
-        <v>1.053769161789848</v>
+        <v>1.018247245402604</v>
       </c>
       <c r="M20">
-        <v>1.066041819645306</v>
+        <v>1.014052326014955</v>
       </c>
       <c r="N20">
-        <v>1.0661482908144</v>
+        <v>1.013006910173542</v>
       </c>
       <c r="O20">
-        <v>1.055329693380364</v>
+        <v>0.9639673182955275</v>
       </c>
       <c r="P20">
-        <v>1.036348867532007</v>
+        <v>0.9870195288378207</v>
       </c>
       <c r="Q20">
-        <v>1.058935892525042</v>
+        <v>0.9803138489215323</v>
       </c>
       <c r="R20">
-        <v>1.076706119973087</v>
+        <v>0.9871386727759132</v>
       </c>
       <c r="S20">
-        <v>1.058935892525042</v>
+        <v>0.9803138489215324</v>
       </c>
       <c r="T20">
-        <v>1.074066662683415</v>
+        <v>0.9936057321253204</v>
       </c>
       <c r="U20">
-        <v>1.072482988309612</v>
+        <v>0.9974859677349647</v>
       </c>
       <c r="V20">
-        <v>1.028575107139494</v>
+        <v>0.98897588942862</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -1943,64 +1946,64 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>1.033676186590325</v>
+        <v>1.0661482908144</v>
       </c>
       <c r="D21">
-        <v>1.016096562553626</v>
+        <v>1.157420624855248</v>
       </c>
       <c r="E21">
-        <v>1.017108734247791</v>
+        <v>0.9532387619054798</v>
       </c>
       <c r="F21">
-        <v>0.9616772178385905</v>
+        <v>1.119458973158533</v>
       </c>
       <c r="G21">
-        <v>1.033676186590325</v>
+        <v>1.0661482908144</v>
       </c>
       <c r="H21">
-        <v>1.016096562553626</v>
+        <v>1.157420624855248</v>
       </c>
       <c r="I21">
-        <v>1.018466373621936</v>
+        <v>0.9258962165137228</v>
       </c>
       <c r="J21">
-        <v>0.9571424806198257</v>
+        <v>0.8128883259974095</v>
       </c>
       <c r="K21">
-        <v>1.000978348976898</v>
+        <v>1.139780502081307</v>
       </c>
       <c r="L21">
-        <v>0.9860157566340269</v>
+        <v>1.053769161789848</v>
       </c>
       <c r="M21">
-        <v>1.033833458978079</v>
+        <v>1.066041819645306</v>
       </c>
       <c r="N21">
-        <v>1.033676186590325</v>
+        <v>1.0661482908144</v>
       </c>
       <c r="O21">
-        <v>1.016602648400708</v>
+        <v>1.055329693380364</v>
       </c>
       <c r="P21">
-        <v>0.9893929760431905</v>
+        <v>1.036348867532007</v>
       </c>
       <c r="Q21">
-        <v>1.022293827797247</v>
+        <v>1.058935892525042</v>
       </c>
       <c r="R21">
-        <v>0.9982941715466692</v>
+        <v>1.076706119973087</v>
       </c>
       <c r="S21">
-        <v>1.022293827797247</v>
+        <v>1.058935892525042</v>
       </c>
       <c r="T21">
-        <v>1.007139675307583</v>
+        <v>1.074066662683415</v>
       </c>
       <c r="U21">
-        <v>1.012446977564131</v>
+        <v>1.072482988309612</v>
       </c>
       <c r="V21">
-        <v>0.9988952076353774</v>
+        <v>1.028575107139494</v>
       </c>
     </row>
     <row r="22" spans="1:22">
@@ -2011,64 +2014,64 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>1.02638175785845</v>
+        <v>1.033676186590325</v>
       </c>
       <c r="D22">
-        <v>1.029895055923129</v>
+        <v>1.016096562553626</v>
       </c>
       <c r="E22">
-        <v>0.9260333993718453</v>
+        <v>1.017108734247791</v>
       </c>
       <c r="F22">
-        <v>0.9664529013989273</v>
+        <v>0.9616772178385905</v>
       </c>
       <c r="G22">
-        <v>1.02638175785845</v>
+        <v>1.033676186590325</v>
       </c>
       <c r="H22">
-        <v>1.029895055923129</v>
+        <v>1.016096562553626</v>
       </c>
       <c r="I22">
-        <v>1.042204701063091</v>
+        <v>1.018466373621936</v>
       </c>
       <c r="J22">
-        <v>0.9341577907095099</v>
+        <v>0.9571424806198257</v>
       </c>
       <c r="K22">
-        <v>1.018335647130066</v>
+        <v>1.000978348976898</v>
       </c>
       <c r="L22">
-        <v>0.9849954260485555</v>
+        <v>0.9860157566340269</v>
       </c>
       <c r="M22">
-        <v>1.027320483489625</v>
+        <v>1.033833458978079</v>
       </c>
       <c r="N22">
-        <v>1.02638175785845</v>
+        <v>1.033676186590325</v>
       </c>
       <c r="O22">
-        <v>0.977964227647487</v>
+        <v>1.016602648400708</v>
       </c>
       <c r="P22">
-        <v>0.9462431503853863</v>
+        <v>0.9893929760431905</v>
       </c>
       <c r="Q22">
-        <v>0.9941034043844749</v>
+        <v>1.022293827797247</v>
       </c>
       <c r="R22">
-        <v>0.9741271188979671</v>
+        <v>0.9982941715466692</v>
       </c>
       <c r="S22">
-        <v>0.9941034043844749</v>
+        <v>1.022293827797247</v>
       </c>
       <c r="T22">
-        <v>0.987190778638088</v>
+        <v>1.007139675307583</v>
       </c>
       <c r="U22">
-        <v>0.9950289744821605</v>
+        <v>1.012446977564131</v>
       </c>
       <c r="V22">
-        <v>0.9910570849379468</v>
+        <v>0.9988952076353774</v>
       </c>
     </row>
     <row r="23" spans="1:22">
@@ -2079,64 +2082,64 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>1.296550259268289</v>
+        <v>1.02638175785845</v>
       </c>
       <c r="D23">
-        <v>1.102317141619031</v>
+        <v>1.029895055923129</v>
       </c>
       <c r="E23">
-        <v>0.6144499547809283</v>
+        <v>0.9260333993718453</v>
       </c>
       <c r="F23">
-        <v>0.9869265953934006</v>
+        <v>0.9664529013989273</v>
       </c>
       <c r="G23">
-        <v>1.296550259268289</v>
+        <v>1.02638175785845</v>
       </c>
       <c r="H23">
-        <v>1.102317141619031</v>
+        <v>1.029895055923129</v>
       </c>
       <c r="I23">
-        <v>0.9436198011709852</v>
+        <v>1.042204701063091</v>
       </c>
       <c r="J23">
-        <v>0.9090622429099344</v>
+        <v>0.9341577907095099</v>
       </c>
       <c r="K23">
-        <v>1.012083775869545</v>
+        <v>1.018335647130066</v>
       </c>
       <c r="L23">
-        <v>1.046713311285708</v>
+        <v>0.9849954260485555</v>
       </c>
       <c r="M23">
-        <v>1.299053527618088</v>
+        <v>1.027320483489625</v>
       </c>
       <c r="N23">
-        <v>1.296550259268289</v>
+        <v>1.02638175785845</v>
       </c>
       <c r="O23">
-        <v>0.8583835481999798</v>
+        <v>0.977964227647487</v>
       </c>
       <c r="P23">
-        <v>0.8006882750871644</v>
+        <v>0.9462431503853863</v>
       </c>
       <c r="Q23">
-        <v>1.004439118556083</v>
+        <v>0.9941034043844749</v>
       </c>
       <c r="R23">
-        <v>0.9012312305977866</v>
+        <v>0.9741271188979671</v>
       </c>
       <c r="S23">
-        <v>1.004439118556083</v>
+        <v>0.9941034043844749</v>
       </c>
       <c r="T23">
-        <v>1.000060987765412</v>
+        <v>0.987190778638088</v>
       </c>
       <c r="U23">
-        <v>1.059358842065988</v>
+        <v>0.9950289744821605</v>
       </c>
       <c r="V23">
-        <v>0.9889653852872277</v>
+        <v>0.9910570849379468</v>
       </c>
     </row>
     <row r="24" spans="1:22">
@@ -2147,64 +2150,64 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>1.182639166750455</v>
+        <v>1.296550259268289</v>
       </c>
       <c r="D24">
-        <v>1.022448556450421</v>
+        <v>1.102317141619031</v>
       </c>
       <c r="E24">
-        <v>0.8468870807590742</v>
+        <v>0.6144499547809283</v>
       </c>
       <c r="F24">
-        <v>1.059349688306665</v>
+        <v>0.9869265953934006</v>
       </c>
       <c r="G24">
-        <v>1.182639166750455</v>
+        <v>1.296550259268289</v>
       </c>
       <c r="H24">
-        <v>1.022448556450421</v>
+        <v>1.102317141619031</v>
       </c>
       <c r="I24">
-        <v>0.9335862693644296</v>
+        <v>0.9436198011709852</v>
       </c>
       <c r="J24">
-        <v>0.8219610519358863</v>
+        <v>0.9090622429099344</v>
       </c>
       <c r="K24">
-        <v>1.163648357294598</v>
+        <v>1.012083775869545</v>
       </c>
       <c r="L24">
-        <v>1.056066471846118</v>
+        <v>1.046713311285708</v>
       </c>
       <c r="M24">
-        <v>1.182639166750455</v>
+        <v>1.299053527618088</v>
       </c>
       <c r="N24">
-        <v>1.182639166750455</v>
+        <v>1.296550259268289</v>
       </c>
       <c r="O24">
-        <v>0.9346678186047477</v>
+        <v>0.8583835481999798</v>
       </c>
       <c r="P24">
-        <v>0.9531183845328697</v>
+        <v>0.8006882750871644</v>
       </c>
       <c r="Q24">
-        <v>1.017324934653317</v>
+        <v>1.004439118556083</v>
       </c>
       <c r="R24">
-        <v>0.9762284418387202</v>
+        <v>0.9012312305977866</v>
       </c>
       <c r="S24">
-        <v>1.017324934653317</v>
+        <v>1.004439118556083</v>
       </c>
       <c r="T24">
-        <v>1.027831123066654</v>
+        <v>1.000060987765412</v>
       </c>
       <c r="U24">
-        <v>1.058792731803414</v>
+        <v>1.059358842065988</v>
       </c>
       <c r="V24">
-        <v>1.010823330338456</v>
+        <v>0.9889653852872277</v>
       </c>
     </row>
     <row r="25" spans="1:22">
@@ -2215,64 +2218,64 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>1.024661761060706</v>
+        <v>1.182639166750455</v>
       </c>
       <c r="D25">
-        <v>1.015583805408982</v>
+        <v>1.022448556450421</v>
       </c>
       <c r="E25">
-        <v>0.9735472749553575</v>
+        <v>0.8468870807590742</v>
       </c>
       <c r="F25">
-        <v>0.9980574595524999</v>
+        <v>1.059349688306665</v>
       </c>
       <c r="G25">
-        <v>1.024661761060706</v>
+        <v>1.182639166750455</v>
       </c>
       <c r="H25">
-        <v>1.015583805408982</v>
+        <v>1.022448556450421</v>
       </c>
       <c r="I25">
-        <v>0.9885609479652178</v>
+        <v>0.9335862693644296</v>
       </c>
       <c r="J25">
-        <v>0.972253858541966</v>
+        <v>0.8219610519358863</v>
       </c>
       <c r="K25">
-        <v>1.00452363658196</v>
+        <v>1.163648357294598</v>
       </c>
       <c r="L25">
-        <v>1.000663628695495</v>
+        <v>1.056066471846118</v>
       </c>
       <c r="M25">
-        <v>1.024665884301018</v>
+        <v>1.182639166750455</v>
       </c>
       <c r="N25">
-        <v>1.024661761060706</v>
+        <v>1.182639166750455</v>
       </c>
       <c r="O25">
-        <v>0.9945655401821698</v>
+        <v>0.9346678186047477</v>
       </c>
       <c r="P25">
-        <v>0.9858023672539287</v>
+        <v>0.9531183845328697</v>
       </c>
       <c r="Q25">
-        <v>1.004597613808349</v>
+        <v>1.017324934653317</v>
       </c>
       <c r="R25">
-        <v>0.9957295133056131</v>
+        <v>0.9762284418387202</v>
       </c>
       <c r="S25">
-        <v>1.004597613808349</v>
+        <v>1.017324934653317</v>
       </c>
       <c r="T25">
-        <v>1.002962575244386</v>
+        <v>1.027831123066654</v>
       </c>
       <c r="U25">
-        <v>1.00730241240765</v>
+        <v>1.058792731803414</v>
       </c>
       <c r="V25">
-        <v>0.997231546595273</v>
+        <v>1.010823330338456</v>
       </c>
     </row>
     <row r="26" spans="1:22">
@@ -2283,64 +2286,64 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>0.9940133776583997</v>
+        <v>1.024661761060706</v>
       </c>
       <c r="D26">
-        <v>0.9931505334879469</v>
+        <v>1.015583805408982</v>
       </c>
       <c r="E26">
-        <v>1.000848245555628</v>
+        <v>0.9735472749553575</v>
       </c>
       <c r="F26">
-        <v>0.9923005744966766</v>
+        <v>0.9980574595524999</v>
       </c>
       <c r="G26">
-        <v>0.9940133776583997</v>
+        <v>1.024661761060706</v>
       </c>
       <c r="H26">
-        <v>0.9931505334879469</v>
+        <v>1.015583805408982</v>
       </c>
       <c r="I26">
-        <v>0.9908835948381052</v>
+        <v>0.9885609479652178</v>
       </c>
       <c r="J26">
-        <v>0.9955886800323198</v>
+        <v>0.972253858541966</v>
       </c>
       <c r="K26">
-        <v>0.9910476314154779</v>
+        <v>1.00452363658196</v>
       </c>
       <c r="L26">
-        <v>0.9906306436038276</v>
+        <v>1.000663628695495</v>
       </c>
       <c r="M26">
-        <v>0.9940249164970888</v>
+        <v>1.024665884301018</v>
       </c>
       <c r="N26">
-        <v>0.9940133776583997</v>
+        <v>1.024661761060706</v>
       </c>
       <c r="O26">
-        <v>0.9969993895217876</v>
+        <v>0.9945655401821698</v>
       </c>
       <c r="P26">
-        <v>0.9965744100261524</v>
+        <v>0.9858023672539287</v>
       </c>
       <c r="Q26">
-        <v>0.9960040522339916</v>
+        <v>1.004597613808349</v>
       </c>
       <c r="R26">
-        <v>0.9954331178467507</v>
+        <v>0.9957295133056131</v>
       </c>
       <c r="S26">
-        <v>0.9960040522339916</v>
+        <v>1.004597613808349</v>
       </c>
       <c r="T26">
-        <v>0.9950781827996629</v>
+        <v>1.002962575244386</v>
       </c>
       <c r="U26">
-        <v>0.9948652217714102</v>
+        <v>1.00730241240765</v>
       </c>
       <c r="V26">
-        <v>0.9935579101360478</v>
+        <v>0.997231546595273</v>
       </c>
     </row>
     <row r="27" spans="1:22">
@@ -2351,64 +2354,64 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>1.074604189628469</v>
+        <v>0.9940133776583997</v>
       </c>
       <c r="D27">
-        <v>1.015201861944802</v>
+        <v>0.9931505334879469</v>
       </c>
       <c r="E27">
-        <v>0.9564332673417275</v>
+        <v>1.000848245555628</v>
       </c>
       <c r="F27">
-        <v>0.9916919887572045</v>
+        <v>0.9923005744966766</v>
       </c>
       <c r="G27">
-        <v>1.074604189628469</v>
+        <v>0.9940133776583997</v>
       </c>
       <c r="H27">
-        <v>1.015201861944802</v>
+        <v>0.9931505334879469</v>
       </c>
       <c r="I27">
-        <v>0.9940261341466884</v>
+        <v>0.9908835948381052</v>
       </c>
       <c r="J27">
-        <v>0.9520241607785629</v>
+        <v>0.9955886800323198</v>
       </c>
       <c r="K27">
-        <v>1.018454516140518</v>
+        <v>0.9910476314154779</v>
       </c>
       <c r="L27">
-        <v>0.9883049179398178</v>
+        <v>0.9906306436038276</v>
       </c>
       <c r="M27">
-        <v>1.074595640962871</v>
+        <v>0.9940249164970888</v>
       </c>
       <c r="N27">
-        <v>1.074604189628469</v>
+        <v>0.9940133776583997</v>
       </c>
       <c r="O27">
-        <v>0.985817564643265</v>
+        <v>0.9969993895217876</v>
       </c>
       <c r="P27">
-        <v>0.974062628049466</v>
+        <v>0.9965744100261524</v>
       </c>
       <c r="Q27">
-        <v>1.015413106305</v>
+        <v>0.9960040522339916</v>
       </c>
       <c r="R27">
-        <v>0.9877757060145781</v>
+        <v>0.9954331178467507</v>
       </c>
       <c r="S27">
-        <v>1.015413106305</v>
+        <v>0.9960040522339916</v>
       </c>
       <c r="T27">
-        <v>1.009482826918051</v>
+        <v>0.9950781827996629</v>
       </c>
       <c r="U27">
-        <v>1.022507099460135</v>
+        <v>0.9948652217714102</v>
       </c>
       <c r="V27">
-        <v>0.9988426295847237</v>
+        <v>0.9935579101360478</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -2419,64 +2422,64 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>1.146050040462977</v>
+        <v>1.074604189628469</v>
       </c>
       <c r="D28">
-        <v>1.111204180838279</v>
+        <v>1.015201861944802</v>
       </c>
       <c r="E28">
-        <v>0.8722932950832084</v>
+        <v>0.9564332673417275</v>
       </c>
       <c r="F28">
-        <v>1.011524781298674</v>
+        <v>0.9916919887572045</v>
       </c>
       <c r="G28">
-        <v>1.146050040462977</v>
+        <v>1.074604189628469</v>
       </c>
       <c r="H28">
-        <v>1.111204180838279</v>
+        <v>1.015201861944802</v>
       </c>
       <c r="I28">
-        <v>0.9553491067657652</v>
+        <v>0.9940261341466884</v>
       </c>
       <c r="J28">
-        <v>0.9195314690695785</v>
+        <v>0.9520241607785629</v>
       </c>
       <c r="K28">
-        <v>1.039124403023922</v>
+        <v>1.018454516140518</v>
       </c>
       <c r="L28">
-        <v>1.031211448460352</v>
+        <v>0.9883049179398178</v>
       </c>
       <c r="M28">
-        <v>1.145956502716261</v>
+        <v>1.074595640962871</v>
       </c>
       <c r="N28">
-        <v>1.146050040462977</v>
+        <v>1.074604189628469</v>
       </c>
       <c r="O28">
-        <v>0.9917487379607435</v>
+        <v>0.985817564643265</v>
       </c>
       <c r="P28">
-        <v>0.941909038190941</v>
+        <v>0.974062628049466</v>
       </c>
       <c r="Q28">
-        <v>1.043182505461488</v>
+        <v>1.015413106305</v>
       </c>
       <c r="R28">
-        <v>0.9983407524067202</v>
+        <v>0.9877757060145781</v>
       </c>
       <c r="S28">
-        <v>1.043182505461488</v>
+        <v>1.015413106305</v>
       </c>
       <c r="T28">
-        <v>1.035268074420785</v>
+        <v>1.009482826918051</v>
       </c>
       <c r="U28">
-        <v>1.057424467629223</v>
+        <v>1.022507099460135</v>
       </c>
       <c r="V28">
-        <v>1.010786090625345</v>
+        <v>0.9988426295847237</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -2487,64 +2490,64 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>1.02484593897323</v>
+        <v>1.146050040462977</v>
       </c>
       <c r="D29">
-        <v>1.015723980959849</v>
+        <v>1.111204180838279</v>
       </c>
       <c r="E29">
-        <v>0.9738394584922864</v>
+        <v>0.8722932950832084</v>
       </c>
       <c r="F29">
-        <v>0.9976436600720405</v>
+        <v>1.011524781298674</v>
       </c>
       <c r="G29">
-        <v>1.02484593897323</v>
+        <v>1.146050040462977</v>
       </c>
       <c r="H29">
-        <v>1.015723980959849</v>
+        <v>1.111204180838279</v>
       </c>
       <c r="I29">
-        <v>0.988378331789019</v>
+        <v>0.9553491067657652</v>
       </c>
       <c r="J29">
-        <v>0.9729076635063872</v>
+        <v>0.9195314690695785</v>
       </c>
       <c r="K29">
-        <v>1.004304578992173</v>
+        <v>1.039124403023922</v>
       </c>
       <c r="L29">
-        <v>1.000119053685809</v>
+        <v>1.031211448460352</v>
       </c>
       <c r="M29">
-        <v>1.024848773657823</v>
+        <v>1.145956502716261</v>
       </c>
       <c r="N29">
-        <v>1.02484593897323</v>
+        <v>1.146050040462977</v>
       </c>
       <c r="O29">
-        <v>0.9947817197260675</v>
+        <v>0.9917487379607435</v>
       </c>
       <c r="P29">
-        <v>0.9857415592821634</v>
+        <v>0.941909038190941</v>
       </c>
       <c r="Q29">
-        <v>1.004803126141788</v>
+        <v>1.043182505461488</v>
       </c>
       <c r="R29">
-        <v>0.9957356998413919</v>
+        <v>0.9983407524067202</v>
       </c>
       <c r="S29">
-        <v>1.004803126141788</v>
+        <v>1.043182505461488</v>
       </c>
       <c r="T29">
-        <v>1.003013259624351</v>
+        <v>1.035268074420785</v>
       </c>
       <c r="U29">
-        <v>1.007379795494127</v>
+        <v>1.057424467629223</v>
       </c>
       <c r="V29">
-        <v>0.9972203333088493</v>
+        <v>1.010786090625345</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -2555,64 +2558,64 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>0.9940544177545264</v>
+        <v>1.02484593897323</v>
       </c>
       <c r="D30">
-        <v>0.9933074094322598</v>
+        <v>1.015723980959849</v>
       </c>
       <c r="E30">
-        <v>1.000964389291533</v>
+        <v>0.9738394584922864</v>
       </c>
       <c r="F30">
-        <v>0.9923462355144899</v>
+        <v>0.9976436600720405</v>
       </c>
       <c r="G30">
-        <v>0.9940544177545264</v>
+        <v>1.02484593897323</v>
       </c>
       <c r="H30">
-        <v>0.9933074094322598</v>
+        <v>1.015723980959849</v>
       </c>
       <c r="I30">
-        <v>0.9908562651504863</v>
+        <v>0.988378331789019</v>
       </c>
       <c r="J30">
-        <v>0.9955743907110319</v>
+        <v>0.9729076635063872</v>
       </c>
       <c r="K30">
-        <v>0.9910225826403489</v>
+        <v>1.004304578992173</v>
       </c>
       <c r="L30">
-        <v>0.9906301811092681</v>
+        <v>1.000119053685809</v>
       </c>
       <c r="M30">
-        <v>0.9940640433116159</v>
+        <v>1.024848773657823</v>
       </c>
       <c r="N30">
-        <v>0.9940544177545264</v>
+        <v>1.02484593897323</v>
       </c>
       <c r="O30">
-        <v>0.9971358993618966</v>
+        <v>0.9947817197260675</v>
       </c>
       <c r="P30">
-        <v>0.9966553124030116</v>
+        <v>0.9857415592821634</v>
       </c>
       <c r="Q30">
-        <v>0.9961087388261065</v>
+        <v>1.004803126141788</v>
       </c>
       <c r="R30">
-        <v>0.9955393447460944</v>
+        <v>0.9957356998413919</v>
       </c>
       <c r="S30">
-        <v>0.9961087388261065</v>
+        <v>1.004803126141788</v>
       </c>
       <c r="T30">
-        <v>0.9951681129982024</v>
+        <v>1.003013259624351</v>
       </c>
       <c r="U30">
-        <v>0.9949453739494671</v>
+        <v>1.007379795494127</v>
       </c>
       <c r="V30">
-        <v>0.9935944839504931</v>
+        <v>0.9972203333088493</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -2623,64 +2626,64 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>1.074007257196432</v>
+        <v>0.9940544177545264</v>
       </c>
       <c r="D31">
-        <v>1.015044245629182</v>
+        <v>0.9933074094322598</v>
       </c>
       <c r="E31">
-        <v>0.9567630915180453</v>
+        <v>1.000964389291533</v>
       </c>
       <c r="F31">
-        <v>0.9912448752842513</v>
+        <v>0.9923462355144899</v>
       </c>
       <c r="G31">
-        <v>1.074007257196432</v>
+        <v>0.9940544177545264</v>
       </c>
       <c r="H31">
-        <v>1.015044245629182</v>
+        <v>0.9933074094322598</v>
       </c>
       <c r="I31">
-        <v>0.9937968403525195</v>
+        <v>0.9908562651504863</v>
       </c>
       <c r="J31">
-        <v>0.9530531379968976</v>
+        <v>0.9955743907110319</v>
       </c>
       <c r="K31">
-        <v>1.018083959883863</v>
+        <v>0.9910225826403489</v>
       </c>
       <c r="L31">
-        <v>0.9877022706377734</v>
+        <v>0.9906301811092681</v>
       </c>
       <c r="M31">
-        <v>1.073998847772522</v>
+        <v>0.9940640433116159</v>
       </c>
       <c r="N31">
-        <v>1.074007257196432</v>
+        <v>0.9940544177545264</v>
       </c>
       <c r="O31">
-        <v>0.9859036685736136</v>
+        <v>0.9971358993618966</v>
       </c>
       <c r="P31">
-        <v>0.9740039834011482</v>
+        <v>0.9966553124030116</v>
       </c>
       <c r="Q31">
-        <v>1.015271531447887</v>
+        <v>0.9961087388261065</v>
       </c>
       <c r="R31">
-        <v>0.9876840708104928</v>
+        <v>0.9955393447460944</v>
       </c>
       <c r="S31">
-        <v>1.015271531447887</v>
+        <v>0.9961087388261065</v>
       </c>
       <c r="T31">
-        <v>1.009264867406978</v>
+        <v>0.9951681129982024</v>
       </c>
       <c r="U31">
-        <v>1.022213345364869</v>
+        <v>0.9949453739494671</v>
       </c>
       <c r="V31">
-        <v>0.9987119598123706</v>
+        <v>0.9935944839504931</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -2691,64 +2694,64 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <v>1.144594173439702</v>
+        <v>1.074007257196432</v>
       </c>
       <c r="D32">
-        <v>1.108719862811576</v>
+        <v>1.015044245629182</v>
       </c>
       <c r="E32">
-        <v>0.8736391964638899</v>
+        <v>0.9567630915180453</v>
       </c>
       <c r="F32">
-        <v>1.010129769856939</v>
+        <v>0.9912448752842513</v>
       </c>
       <c r="G32">
-        <v>1.144594173439702</v>
+        <v>1.074007257196432</v>
       </c>
       <c r="H32">
-        <v>1.108719862811576</v>
+        <v>1.015044245629182</v>
       </c>
       <c r="I32">
-        <v>0.955731013115665</v>
+        <v>0.9937968403525195</v>
       </c>
       <c r="J32">
-        <v>0.9213072569316975</v>
+        <v>0.9530531379968976</v>
       </c>
       <c r="K32">
-        <v>1.038436975122679</v>
+        <v>1.018083959883863</v>
       </c>
       <c r="L32">
-        <v>1.029997185359806</v>
+        <v>0.9877022706377734</v>
       </c>
       <c r="M32">
-        <v>1.144499647850914</v>
+        <v>1.073998847772522</v>
       </c>
       <c r="N32">
-        <v>1.144594173439702</v>
+        <v>1.074007257196432</v>
       </c>
       <c r="O32">
-        <v>0.9911795296377328</v>
+        <v>0.9859036685736136</v>
       </c>
       <c r="P32">
-        <v>0.9418844831604144</v>
+        <v>0.9740039834011482</v>
       </c>
       <c r="Q32">
-        <v>1.04231774423839</v>
+        <v>1.015271531447887</v>
       </c>
       <c r="R32">
-        <v>0.9974962763774681</v>
+        <v>0.9876840708104928</v>
       </c>
       <c r="S32">
-        <v>1.042317744238389</v>
+        <v>1.015271531447887</v>
       </c>
       <c r="T32">
-        <v>1.034270750643027</v>
+        <v>1.009264867406978</v>
       </c>
       <c r="U32">
-        <v>1.056335435202362</v>
+        <v>1.022213345364869</v>
       </c>
       <c r="V32">
-        <v>1.010319429137744</v>
+        <v>0.9987119598123706</v>
       </c>
     </row>
     <row r="33" spans="1:22">
@@ -2759,64 +2762,64 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <v>1.024849952889729</v>
+        <v>1.144594173439702</v>
       </c>
       <c r="D33">
-        <v>1.015533013343277</v>
+        <v>1.108719862811576</v>
       </c>
       <c r="E33">
-        <v>0.974558034205984</v>
+        <v>0.8736391964638899</v>
       </c>
       <c r="F33">
-        <v>0.9960405202315471</v>
+        <v>1.010129769856939</v>
       </c>
       <c r="G33">
-        <v>1.024849952889729</v>
+        <v>1.144594173439702</v>
       </c>
       <c r="H33">
-        <v>1.015533013343277</v>
+        <v>1.108719862811576</v>
       </c>
       <c r="I33">
-        <v>0.9877695741113146</v>
+        <v>0.955731013115665</v>
       </c>
       <c r="J33">
-        <v>0.9756398889565583</v>
+        <v>0.9213072569316975</v>
       </c>
       <c r="K33">
-        <v>1.003456637153429</v>
+        <v>1.038436975122679</v>
       </c>
       <c r="L33">
-        <v>0.9981236121041758</v>
+        <v>1.029997185359806</v>
       </c>
       <c r="M33">
-        <v>1.024843383608217</v>
+        <v>1.144499647850914</v>
       </c>
       <c r="N33">
-        <v>1.024849952889729</v>
+        <v>1.144594173439702</v>
       </c>
       <c r="O33">
-        <v>0.9950455237746303</v>
+        <v>0.9911795296377328</v>
       </c>
       <c r="P33">
-        <v>0.9852992772187655</v>
+        <v>0.9418844831604144</v>
       </c>
       <c r="Q33">
-        <v>1.004980333479663</v>
+        <v>1.04231774423839</v>
       </c>
       <c r="R33">
-        <v>0.9953771892602692</v>
+        <v>0.9974962763774681</v>
       </c>
       <c r="S33">
-        <v>1.004980333479663</v>
+        <v>1.042317744238389</v>
       </c>
       <c r="T33">
-        <v>1.002745380167634</v>
+        <v>1.034270750643027</v>
       </c>
       <c r="U33">
-        <v>1.007166294712053</v>
+        <v>1.056335435202362</v>
       </c>
       <c r="V33">
-        <v>0.9969964041245019</v>
+        <v>1.010319429137744</v>
       </c>
     </row>
     <row r="34" spans="1:22">
@@ -2827,64 +2830,64 @@
         <v>32</v>
       </c>
       <c r="C34">
-        <v>0.9939501578815271</v>
+        <v>1.024849952889729</v>
       </c>
       <c r="D34">
-        <v>0.9935401072533991</v>
+        <v>1.015533013343277</v>
       </c>
       <c r="E34">
-        <v>1.001064435729022</v>
+        <v>0.974558034205984</v>
       </c>
       <c r="F34">
-        <v>0.9923232829766724</v>
+        <v>0.9960405202315471</v>
       </c>
       <c r="G34">
-        <v>0.9939501578815271</v>
+        <v>1.024849952889729</v>
       </c>
       <c r="H34">
-        <v>0.9935401072533991</v>
+        <v>1.015533013343277</v>
       </c>
       <c r="I34">
-        <v>0.9906552654996791</v>
+        <v>0.9877695741113146</v>
       </c>
       <c r="J34">
-        <v>0.9959087104142533</v>
+        <v>0.9756398889565583</v>
       </c>
       <c r="K34">
-        <v>0.9908945661483495</v>
+        <v>1.003456637153429</v>
       </c>
       <c r="L34">
-        <v>0.9905466539511947</v>
+        <v>0.9981236121041758</v>
       </c>
       <c r="M34">
-        <v>0.993945377024507</v>
+        <v>1.024843383608217</v>
       </c>
       <c r="N34">
-        <v>0.9939501578815271</v>
+        <v>1.024849952889729</v>
       </c>
       <c r="O34">
-        <v>0.9973022714912104</v>
+        <v>0.9950455237746303</v>
       </c>
       <c r="P34">
-        <v>0.996693859352847</v>
+        <v>0.9852992772187655</v>
       </c>
       <c r="Q34">
-        <v>0.9961849002879827</v>
+        <v>1.004980333479663</v>
       </c>
       <c r="R34">
-        <v>0.9956426086530311</v>
+        <v>0.9953771892602692</v>
       </c>
       <c r="S34">
-        <v>0.9961849002879827</v>
+        <v>1.004980333479663</v>
       </c>
       <c r="T34">
-        <v>0.995219495960155</v>
+        <v>1.002745380167634</v>
       </c>
       <c r="U34">
-        <v>0.9949656283444295</v>
+        <v>1.007166294712053</v>
       </c>
       <c r="V34">
-        <v>0.9936103974817621</v>
+        <v>0.9969964041245019</v>
       </c>
     </row>
     <row r="35" spans="1:22">
@@ -2895,64 +2898,64 @@
         <v>33</v>
       </c>
       <c r="C35">
-        <v>1.071306461914704</v>
+        <v>0.9939501578815271</v>
       </c>
       <c r="D35">
-        <v>1.013578154413121</v>
+        <v>0.9935401072533991</v>
       </c>
       <c r="E35">
-        <v>0.9572031917349948</v>
+        <v>1.001064435729022</v>
       </c>
       <c r="F35">
-        <v>0.9893305674620152</v>
+        <v>0.9923232829766724</v>
       </c>
       <c r="G35">
-        <v>1.071306461914704</v>
+        <v>0.9939501578815271</v>
       </c>
       <c r="H35">
-        <v>1.013578154413121</v>
+        <v>0.9935401072533991</v>
       </c>
       <c r="I35">
-        <v>0.9932346460451377</v>
+        <v>0.9906552654996791</v>
       </c>
       <c r="J35">
-        <v>0.9573211516287912</v>
+        <v>0.9959087104142533</v>
       </c>
       <c r="K35">
-        <v>1.016451985916431</v>
+        <v>0.9908945661483495</v>
       </c>
       <c r="L35">
-        <v>0.9854838804406567</v>
+        <v>0.9905466539511947</v>
       </c>
       <c r="M35">
-        <v>1.0712960022033</v>
+        <v>0.993945377024507</v>
       </c>
       <c r="N35">
-        <v>1.071306461914704</v>
+        <v>0.9939501578815271</v>
       </c>
       <c r="O35">
-        <v>0.9853906730740581</v>
+        <v>0.9973022714912104</v>
       </c>
       <c r="P35">
-        <v>0.973266879598505</v>
+        <v>0.996693859352847</v>
       </c>
       <c r="Q35">
-        <v>1.014029269354273</v>
+        <v>0.9961849002879827</v>
       </c>
       <c r="R35">
-        <v>0.9867039712033772</v>
+        <v>0.9956426086530311</v>
       </c>
       <c r="S35">
-        <v>1.014029269354273</v>
+        <v>0.9961849002879827</v>
       </c>
       <c r="T35">
-        <v>1.007854593881209</v>
+        <v>0.995219495960155</v>
       </c>
       <c r="U35">
-        <v>1.020544967487908</v>
+        <v>0.9949656283444295</v>
       </c>
       <c r="V35">
-        <v>0.9979887549444815</v>
+        <v>0.9936103974817621</v>
       </c>
     </row>
     <row r="36" spans="1:22">
@@ -2963,64 +2966,64 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <v>1.137183521123803</v>
+        <v>1.071306461914704</v>
       </c>
       <c r="D36">
-        <v>1.097864420300833</v>
+        <v>1.013578154413121</v>
       </c>
       <c r="E36">
-        <v>0.8786911853679487</v>
+        <v>0.9572031917349948</v>
       </c>
       <c r="F36">
-        <v>1.004805147670221</v>
+        <v>0.9893305674620152</v>
       </c>
       <c r="G36">
-        <v>1.137183521123803</v>
+        <v>1.071306461914704</v>
       </c>
       <c r="H36">
-        <v>1.097864420300833</v>
+        <v>1.013578154413121</v>
       </c>
       <c r="I36">
-        <v>0.9574342068910251</v>
+        <v>0.9932346460451377</v>
       </c>
       <c r="J36">
-        <v>0.9283831901714723</v>
+        <v>0.9573211516287912</v>
       </c>
       <c r="K36">
-        <v>1.035578566885142</v>
+        <v>1.016451985916431</v>
       </c>
       <c r="L36">
-        <v>1.025168711523754</v>
+        <v>0.9854838804406567</v>
       </c>
       <c r="M36">
-        <v>1.137086928785103</v>
+        <v>1.0712960022033</v>
       </c>
       <c r="N36">
-        <v>1.137183521123803</v>
+        <v>1.071306461914704</v>
       </c>
       <c r="O36">
-        <v>0.9882778028343908</v>
+        <v>0.9853906730740581</v>
       </c>
       <c r="P36">
-        <v>0.941748166519085</v>
+        <v>0.973266879598505</v>
       </c>
       <c r="Q36">
-        <v>1.037913042264195</v>
+        <v>1.014029269354273</v>
       </c>
       <c r="R36">
-        <v>0.9937869177796678</v>
+        <v>0.9867039712033772</v>
       </c>
       <c r="S36">
-        <v>1.037913042264195</v>
+        <v>1.014029269354273</v>
       </c>
       <c r="T36">
-        <v>1.029636068615702</v>
+        <v>1.007854593881209</v>
       </c>
       <c r="U36">
-        <v>1.051145559117322</v>
+        <v>1.020544967487908</v>
       </c>
       <c r="V36">
-        <v>1.008138618741775</v>
+        <v>0.9979887549444815</v>
       </c>
     </row>
     <row r="37" spans="1:22">
@@ -3031,64 +3034,64 @@
         <v>35</v>
       </c>
       <c r="C37">
-        <v>1.024636228731597</v>
+        <v>1.137183521123803</v>
       </c>
       <c r="D37">
-        <v>1.015566889950607</v>
+        <v>1.097864420300833</v>
       </c>
       <c r="E37">
-        <v>0.9735163536699831</v>
+        <v>0.8786911853679487</v>
       </c>
       <c r="F37">
-        <v>0.9981121424462779</v>
+        <v>1.004805147670221</v>
       </c>
       <c r="G37">
-        <v>1.024636228731597</v>
+        <v>1.137183521123803</v>
       </c>
       <c r="H37">
-        <v>1.015566889950607</v>
+        <v>1.097864420300833</v>
       </c>
       <c r="I37">
-        <v>0.9885839440352069</v>
+        <v>0.9574342068910251</v>
       </c>
       <c r="J37">
-        <v>0.9721757552128684</v>
+        <v>0.9283831901714723</v>
       </c>
       <c r="K37">
-        <v>1.004545759768211</v>
+        <v>1.035578566885142</v>
       </c>
       <c r="L37">
-        <v>1.00072602471827</v>
+        <v>1.025168711523754</v>
       </c>
       <c r="M37">
-        <v>1.024640416458755</v>
+        <v>1.137086928785103</v>
       </c>
       <c r="N37">
-        <v>1.024636228731597</v>
+        <v>1.137183521123803</v>
       </c>
       <c r="O37">
-        <v>0.994541621810295</v>
+        <v>0.9882778028343908</v>
       </c>
       <c r="P37">
-        <v>0.9858142480581304</v>
+        <v>0.941748166519085</v>
       </c>
       <c r="Q37">
-        <v>1.004573157450729</v>
+        <v>1.037913042264195</v>
       </c>
       <c r="R37">
-        <v>0.9957317953556227</v>
+        <v>0.9937869177796678</v>
       </c>
       <c r="S37">
-        <v>1.004573157450729</v>
+        <v>1.037913042264195</v>
       </c>
       <c r="T37">
-        <v>1.002957903699616</v>
+        <v>1.029636068615702</v>
       </c>
       <c r="U37">
-        <v>1.007293568706012</v>
+        <v>1.051145559117322</v>
       </c>
       <c r="V37">
-        <v>0.9972328873166276</v>
+        <v>1.008138618741775</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -3099,64 +3102,64 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <v>0.9940096305456401</v>
+        <v>1.024636228731597</v>
       </c>
       <c r="D38">
-        <v>0.9931358089199559</v>
+        <v>1.015566889950607</v>
       </c>
       <c r="E38">
-        <v>1.000837861103138</v>
+        <v>0.9735163536699831</v>
       </c>
       <c r="F38">
-        <v>0.9923003057100891</v>
+        <v>0.9981121424462779</v>
       </c>
       <c r="G38">
-        <v>0.9940096305456401</v>
+        <v>1.024636228731597</v>
       </c>
       <c r="H38">
-        <v>0.9931358089199559</v>
+        <v>1.015566889950607</v>
       </c>
       <c r="I38">
-        <v>0.990887449510466</v>
+        <v>0.9885839440352069</v>
       </c>
       <c r="J38">
-        <v>0.9955891219595527</v>
+        <v>0.9721757552128684</v>
       </c>
       <c r="K38">
-        <v>0.9910475502699322</v>
+        <v>1.004545759768211</v>
       </c>
       <c r="L38">
-        <v>0.9906294195783909</v>
+        <v>1.00072602471827</v>
       </c>
       <c r="M38">
-        <v>0.9940212859089468</v>
+        <v>1.024640416458755</v>
       </c>
       <c r="N38">
-        <v>0.9940096305456401</v>
+        <v>1.024636228731597</v>
       </c>
       <c r="O38">
-        <v>0.9969868350115469</v>
+        <v>0.994541621810295</v>
       </c>
       <c r="P38">
-        <v>0.9965690834066134</v>
+        <v>0.9858142480581304</v>
       </c>
       <c r="Q38">
-        <v>0.9959944335229114</v>
+        <v>1.004573157450729</v>
       </c>
       <c r="R38">
-        <v>0.9954246585777277</v>
+        <v>0.9957317953556227</v>
       </c>
       <c r="S38">
-        <v>0.9959944335229113</v>
+        <v>1.004573157450729</v>
       </c>
       <c r="T38">
-        <v>0.9950709015697057</v>
+        <v>1.002957903699616</v>
       </c>
       <c r="U38">
-        <v>0.9948586473648925</v>
+        <v>1.007293568706012</v>
       </c>
       <c r="V38">
-        <v>0.9935546434496456</v>
+        <v>0.9972328873166276</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -3167,64 +3170,64 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>1.074667032211437</v>
+        <v>0.9940096305456401</v>
       </c>
       <c r="D39">
-        <v>1.015219410002702</v>
+        <v>0.9931358089199559</v>
       </c>
       <c r="E39">
-        <v>0.9564079377099887</v>
+        <v>1.000837861103138</v>
       </c>
       <c r="F39">
-        <v>0.9917557897090546</v>
+        <v>0.9923003057100891</v>
       </c>
       <c r="G39">
-        <v>1.074667032211437</v>
+        <v>0.9940096305456401</v>
       </c>
       <c r="H39">
-        <v>1.015219410002702</v>
+        <v>0.9931358089199559</v>
       </c>
       <c r="I39">
-        <v>0.994047248239174</v>
+        <v>0.990887449510466</v>
       </c>
       <c r="J39">
-        <v>0.9519049732800685</v>
+        <v>0.9955891219595527</v>
       </c>
       <c r="K39">
-        <v>1.018496624448845</v>
+        <v>0.9910475502699322</v>
       </c>
       <c r="L39">
-        <v>0.9883763817032607</v>
+        <v>0.9906294195783909</v>
       </c>
       <c r="M39">
-        <v>1.074658448240363</v>
+        <v>0.9940212859089468</v>
       </c>
       <c r="N39">
-        <v>1.074667032211437</v>
+        <v>0.9940096305456401</v>
       </c>
       <c r="O39">
-        <v>0.9858136738563454</v>
+        <v>0.9969868350115469</v>
       </c>
       <c r="P39">
-        <v>0.9740818637095217</v>
+        <v>0.9965690834066134</v>
       </c>
       <c r="Q39">
-        <v>1.015431459974709</v>
+        <v>0.9959944335229114</v>
       </c>
       <c r="R39">
-        <v>0.9877943791405818</v>
+        <v>0.9954246585777277</v>
       </c>
       <c r="S39">
-        <v>1.015431459974709</v>
+        <v>0.9959944335229113</v>
       </c>
       <c r="T39">
-        <v>1.009512542408296</v>
+        <v>0.9950709015697057</v>
       </c>
       <c r="U39">
-        <v>1.022543440368924</v>
+        <v>0.9948586473648925</v>
       </c>
       <c r="V39">
-        <v>0.9988594246630663</v>
+        <v>0.9935546434496456</v>
       </c>
     </row>
     <row r="40" spans="1:22">
@@ -3235,64 +3238,64 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <v>1.146215578577837</v>
+        <v>1.074667032211437</v>
       </c>
       <c r="D40">
-        <v>1.111494746901827</v>
+        <v>1.015219410002702</v>
       </c>
       <c r="E40">
-        <v>0.8721407931473877</v>
+        <v>0.9564079377099887</v>
       </c>
       <c r="F40">
-        <v>1.01169789348693</v>
+        <v>0.9917557897090546</v>
       </c>
       <c r="G40">
-        <v>1.146215578577837</v>
+        <v>1.074667032211437</v>
       </c>
       <c r="H40">
-        <v>1.111494746901827</v>
+        <v>1.015219410002702</v>
       </c>
       <c r="I40">
-        <v>0.9553035796776486</v>
+        <v>0.994047248239174</v>
       </c>
       <c r="J40">
-        <v>0.9193298874808743</v>
+        <v>0.9519049732800685</v>
       </c>
       <c r="K40">
-        <v>1.039201074657209</v>
+        <v>1.018496624448845</v>
       </c>
       <c r="L40">
-        <v>1.031354950144898</v>
+        <v>0.9883763817032607</v>
       </c>
       <c r="M40">
-        <v>1.14612215213478</v>
+        <v>1.074658448240363</v>
       </c>
       <c r="N40">
-        <v>1.146215578577837</v>
+        <v>1.074667032211437</v>
       </c>
       <c r="O40">
-        <v>0.9918177700246076</v>
+        <v>0.9858136738563454</v>
       </c>
       <c r="P40">
-        <v>0.9419193433171588</v>
+        <v>0.9740818637095217</v>
       </c>
       <c r="Q40">
-        <v>1.043283706209017</v>
+        <v>1.015431459974709</v>
       </c>
       <c r="R40">
-        <v>0.9984444778453817</v>
+        <v>0.9877943791405818</v>
       </c>
       <c r="S40">
-        <v>1.043283706209017</v>
+        <v>1.015431459974709</v>
       </c>
       <c r="T40">
-        <v>1.035387253028496</v>
+        <v>1.009512542408296</v>
       </c>
       <c r="U40">
-        <v>1.057552918138364</v>
+        <v>1.022543440368924</v>
       </c>
       <c r="V40">
-        <v>1.010842313009326</v>
+        <v>0.9988594246630663</v>
       </c>
     </row>
     <row r="41" spans="1:22">
@@ -3303,64 +3306,64 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <v>1.025017733832033</v>
+        <v>1.146215578577837</v>
       </c>
       <c r="D41">
-        <v>1.015797169043875</v>
+        <v>1.111494746901827</v>
       </c>
       <c r="E41">
-        <v>0.9741358682488149</v>
+        <v>0.8721407931473877</v>
       </c>
       <c r="F41">
-        <v>0.9969011234740235</v>
+        <v>1.01169789348693</v>
       </c>
       <c r="G41">
-        <v>1.025017733832033</v>
+        <v>1.146215578577837</v>
       </c>
       <c r="H41">
-        <v>1.015797169043875</v>
+        <v>1.111494746901827</v>
       </c>
       <c r="I41">
-        <v>0.9881244952705625</v>
+        <v>0.9553035796776486</v>
       </c>
       <c r="J41">
-        <v>0.9741435403331739</v>
+        <v>0.9193298874808743</v>
       </c>
       <c r="K41">
-        <v>1.003866870824574</v>
+        <v>1.039201074657209</v>
       </c>
       <c r="L41">
-        <v>0.9992067168694531</v>
+        <v>1.031354950144898</v>
       </c>
       <c r="M41">
-        <v>1.025015189351555</v>
+        <v>1.14612215213478</v>
       </c>
       <c r="N41">
-        <v>1.025017733832033</v>
+        <v>1.146215578577837</v>
       </c>
       <c r="O41">
-        <v>0.9949665186463452</v>
+        <v>0.9918177700246076</v>
       </c>
       <c r="P41">
-        <v>0.9855184958614192</v>
+        <v>0.9419193433171588</v>
       </c>
       <c r="Q41">
-        <v>1.004983590374908</v>
+        <v>1.043283706209017</v>
       </c>
       <c r="R41">
-        <v>0.9956113869222379</v>
+        <v>0.9984444778453817</v>
       </c>
       <c r="S41">
-        <v>1.004983590374908</v>
+        <v>1.043283706209017</v>
       </c>
       <c r="T41">
-        <v>1.002962973649687</v>
+        <v>1.035387253028496</v>
       </c>
       <c r="U41">
-        <v>1.007373925686156</v>
+        <v>1.057552918138364</v>
       </c>
       <c r="V41">
-        <v>0.9971491897370639</v>
+        <v>1.010842313009326</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -3371,64 +3374,64 @@
         <v>40</v>
       </c>
       <c r="C42">
-        <v>0.9941644479267049</v>
+        <v>1.025017733832033</v>
       </c>
       <c r="D42">
-        <v>0.9935214902905787</v>
+        <v>1.015797169043875</v>
       </c>
       <c r="E42">
-        <v>1.000930509458619</v>
+        <v>0.9741358682488149</v>
       </c>
       <c r="F42">
-        <v>0.9923215650172452</v>
+        <v>0.9969011234740235</v>
       </c>
       <c r="G42">
-        <v>0.9941644479267049</v>
+        <v>1.025017733832033</v>
       </c>
       <c r="H42">
-        <v>0.9935214902905787</v>
+        <v>1.015797169043875</v>
       </c>
       <c r="I42">
-        <v>0.9908257170170995</v>
+        <v>0.9881244952705625</v>
       </c>
       <c r="J42">
-        <v>0.9957232955565063</v>
+        <v>0.9741435403331739</v>
       </c>
       <c r="K42">
-        <v>0.9908872529051965</v>
+        <v>1.003866870824574</v>
       </c>
       <c r="L42">
-        <v>0.9906086556438858</v>
+        <v>0.9992067168694531</v>
       </c>
       <c r="M42">
-        <v>0.9941659958179595</v>
+        <v>1.025015189351555</v>
       </c>
       <c r="N42">
-        <v>0.9941644479267049</v>
+        <v>1.025017733832033</v>
       </c>
       <c r="O42">
-        <v>0.9972259998745988</v>
+        <v>0.9949665186463452</v>
       </c>
       <c r="P42">
-        <v>0.9966260372379321</v>
+        <v>0.9855184958614192</v>
       </c>
       <c r="Q42">
-        <v>0.9962054825586342</v>
+        <v>1.004983590374908</v>
       </c>
       <c r="R42">
-        <v>0.995591188255481</v>
+        <v>0.9956113869222379</v>
       </c>
       <c r="S42">
-        <v>0.9962054825586342</v>
+        <v>1.004983590374908</v>
       </c>
       <c r="T42">
-        <v>0.995234503173287</v>
+        <v>1.002962973649687</v>
       </c>
       <c r="U42">
-        <v>0.9950204921239706</v>
+        <v>1.007373925686156</v>
       </c>
       <c r="V42">
-        <v>0.9936228667269795</v>
+        <v>0.9971491897370639</v>
       </c>
     </row>
     <row r="43" spans="1:22">
@@ -3439,64 +3442,64 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <v>1.072944008437529</v>
+        <v>0.9941644479267049</v>
       </c>
       <c r="D43">
-        <v>1.014593655600692</v>
+        <v>0.9935214902905787</v>
       </c>
       <c r="E43">
-        <v>0.9569658106237695</v>
+        <v>1.000930509458619</v>
       </c>
       <c r="F43">
-        <v>0.9903758115181132</v>
+        <v>0.9923215650172452</v>
       </c>
       <c r="G43">
-        <v>1.072944008437529</v>
+        <v>0.9941644479267049</v>
       </c>
       <c r="H43">
-        <v>1.014593655600692</v>
+        <v>0.9935214902905787</v>
       </c>
       <c r="I43">
-        <v>0.9934939855733841</v>
+        <v>0.9908257170170995</v>
       </c>
       <c r="J43">
-        <v>0.9550060612237777</v>
+        <v>0.9957232955565063</v>
       </c>
       <c r="K43">
-        <v>1.017315621122897</v>
+        <v>0.9908872529051965</v>
       </c>
       <c r="L43">
-        <v>0.9867144409085931</v>
+        <v>0.9906086556438858</v>
       </c>
       <c r="M43">
-        <v>1.072933529424263</v>
+        <v>0.9941659958179595</v>
       </c>
       <c r="N43">
-        <v>1.072944008437529</v>
+        <v>0.9941644479267049</v>
       </c>
       <c r="O43">
-        <v>0.9857797331122305</v>
+        <v>0.9972259998745988</v>
       </c>
       <c r="P43">
-        <v>0.9736708110709413</v>
+        <v>0.9966260372379321</v>
       </c>
       <c r="Q43">
-        <v>1.014834491553996</v>
+        <v>0.9962054825586342</v>
       </c>
       <c r="R43">
-        <v>0.9873117592475248</v>
+        <v>0.995591188255481</v>
       </c>
       <c r="S43">
-        <v>1.014834491553996</v>
+        <v>0.9962054825586342</v>
       </c>
       <c r="T43">
-        <v>1.008719821545026</v>
+        <v>0.995234503173287</v>
       </c>
       <c r="U43">
-        <v>1.021564658923526</v>
+        <v>0.9950204921239706</v>
       </c>
       <c r="V43">
-        <v>0.9984261743760943</v>
+        <v>0.9936228667269795</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -3507,64 +3510,64 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>1.141538487305878</v>
+        <v>1.072944008437529</v>
       </c>
       <c r="D44">
-        <v>1.104117245377213</v>
+        <v>1.014593655600692</v>
       </c>
       <c r="E44">
-        <v>0.8757570122273639</v>
+        <v>0.9569658106237695</v>
       </c>
       <c r="F44">
-        <v>1.007658338693166</v>
+        <v>0.9903758115181132</v>
       </c>
       <c r="G44">
-        <v>1.141538487305878</v>
+        <v>1.072944008437529</v>
       </c>
       <c r="H44">
-        <v>1.104117245377213</v>
+        <v>1.014593655600692</v>
       </c>
       <c r="I44">
-        <v>0.9564784737304212</v>
+        <v>0.9934939855733841</v>
       </c>
       <c r="J44">
-        <v>0.924583729217297</v>
+        <v>0.9550060612237777</v>
       </c>
       <c r="K44">
-        <v>1.037135068497595</v>
+        <v>1.017315621122897</v>
       </c>
       <c r="L44">
-        <v>1.027901547441084</v>
+        <v>0.9867144409085931</v>
       </c>
       <c r="M44">
-        <v>1.141440943138183</v>
+        <v>1.072933529424263</v>
       </c>
       <c r="N44">
-        <v>1.141538487305878</v>
+        <v>1.072944008437529</v>
       </c>
       <c r="O44">
-        <v>0.9899371288022886</v>
+        <v>0.9857797331122305</v>
       </c>
       <c r="P44">
-        <v>0.941707675460265</v>
+        <v>0.9736708110709413</v>
       </c>
       <c r="Q44">
-        <v>1.040470914970152</v>
+        <v>1.014834491553996</v>
       </c>
       <c r="R44">
-        <v>0.9958441987659145</v>
+        <v>0.9873117592475248</v>
       </c>
       <c r="S44">
-        <v>1.040470914970152</v>
+        <v>1.014834491553996</v>
       </c>
       <c r="T44">
-        <v>1.032267770900905</v>
+        <v>1.008719821545026</v>
       </c>
       <c r="U44">
-        <v>1.0541219141819</v>
+        <v>1.021564658923526</v>
       </c>
       <c r="V44">
-        <v>1.009396237811252</v>
+        <v>0.9984261743760943</v>
       </c>
     </row>
     <row r="45" spans="1:22">
@@ -3575,64 +3578,64 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>1.024808713275692</v>
+        <v>1.141538487305878</v>
       </c>
       <c r="D45">
-        <v>1.015362844837698</v>
+        <v>1.104117245377213</v>
       </c>
       <c r="E45">
-        <v>0.9746813046634366</v>
+        <v>0.8757570122273639</v>
       </c>
       <c r="F45">
-        <v>0.99578154558289</v>
+        <v>1.007658338693166</v>
       </c>
       <c r="G45">
-        <v>1.024808713275692</v>
+        <v>1.141538487305878</v>
       </c>
       <c r="H45">
-        <v>1.015362844837698</v>
+        <v>1.104117245377213</v>
       </c>
       <c r="I45">
-        <v>0.9876979953493562</v>
+        <v>0.9564784737304212</v>
       </c>
       <c r="J45">
-        <v>0.9760382121631204</v>
+        <v>0.924583729217297</v>
       </c>
       <c r="K45">
-        <v>1.003325030477233</v>
+        <v>1.037135068497595</v>
       </c>
       <c r="L45">
-        <v>0.9977965773811608</v>
+        <v>1.027901547441084</v>
       </c>
       <c r="M45">
-        <v>1.024801495641219</v>
+        <v>1.141440943138183</v>
       </c>
       <c r="N45">
-        <v>1.024808713275692</v>
+        <v>1.141538487305878</v>
       </c>
       <c r="O45">
-        <v>0.9950220747505674</v>
+        <v>0.9899371288022886</v>
       </c>
       <c r="P45">
-        <v>0.9852314251231633</v>
+        <v>0.941707675460265</v>
       </c>
       <c r="Q45">
-        <v>1.004950954258942</v>
+        <v>1.040470914970152</v>
       </c>
       <c r="R45">
-        <v>0.9952752316946749</v>
+        <v>0.9958441987659145</v>
       </c>
       <c r="S45">
-        <v>1.004950954258942</v>
+        <v>1.040470914970152</v>
       </c>
       <c r="T45">
-        <v>1.002658602089929</v>
+        <v>1.032267770900905</v>
       </c>
       <c r="U45">
-        <v>1.007088624327082</v>
+        <v>1.0541219141819</v>
       </c>
       <c r="V45">
-        <v>0.9969365279663234</v>
+        <v>1.009396237811252</v>
       </c>
     </row>
     <row r="46" spans="1:22">
@@ -3643,64 +3646,64 @@
         <v>44</v>
       </c>
       <c r="C46">
-        <v>0.9939120451665983</v>
+        <v>1.024808713275692</v>
       </c>
       <c r="D46">
-        <v>0.993435660773743</v>
+        <v>1.015362844837698</v>
       </c>
       <c r="E46">
-        <v>1.001115569860185</v>
+        <v>0.9746813046634366</v>
       </c>
       <c r="F46">
-        <v>0.9922848615898929</v>
+        <v>0.99578154558289</v>
       </c>
       <c r="G46">
-        <v>0.9939120451665983</v>
+        <v>1.024808713275692</v>
       </c>
       <c r="H46">
-        <v>0.993435660773743</v>
+        <v>1.015362844837698</v>
       </c>
       <c r="I46">
-        <v>0.9906469215535926</v>
+        <v>0.9876979953493562</v>
       </c>
       <c r="J46">
-        <v>0.9959513031813313</v>
+        <v>0.9760382121631204</v>
       </c>
       <c r="K46">
-        <v>0.9908615863341106</v>
+        <v>1.003325030477233</v>
       </c>
       <c r="L46">
-        <v>0.9904813140095031</v>
+        <v>0.9977965773811608</v>
       </c>
       <c r="M46">
-        <v>0.9939061735181346</v>
+        <v>1.024801495641219</v>
       </c>
       <c r="N46">
-        <v>0.9939120451665983</v>
+        <v>1.024808713275692</v>
       </c>
       <c r="O46">
-        <v>0.9972756153169642</v>
+        <v>0.9950220747505674</v>
       </c>
       <c r="P46">
-        <v>0.9967002157250392</v>
+        <v>0.9852314251231633</v>
       </c>
       <c r="Q46">
-        <v>0.9961544252668423</v>
+        <v>1.004950954258942</v>
       </c>
       <c r="R46">
-        <v>0.9956120307412738</v>
+        <v>0.9952752316946749</v>
       </c>
       <c r="S46">
-        <v>0.9961544252668423</v>
+        <v>1.004950954258942</v>
       </c>
       <c r="T46">
-        <v>0.9951870343476049</v>
+        <v>1.002658602089929</v>
       </c>
       <c r="U46">
-        <v>0.9949320365114035</v>
+        <v>1.007088624327082</v>
       </c>
       <c r="V46">
-        <v>0.9935861578086196</v>
+        <v>0.9969365279663234</v>
       </c>
     </row>
     <row r="47" spans="1:22">
@@ -3711,64 +3714,64 @@
         <v>45</v>
       </c>
       <c r="C47">
-        <v>1.070764926170405</v>
+        <v>0.9939120451665983</v>
       </c>
       <c r="D47">
-        <v>1.013175312539491</v>
+        <v>0.993435660773743</v>
       </c>
       <c r="E47">
-        <v>0.9572794427580701</v>
+        <v>1.001115569860185</v>
       </c>
       <c r="F47">
-        <v>0.9890453005990636</v>
+        <v>0.9922848615898929</v>
       </c>
       <c r="G47">
-        <v>1.070764926170405</v>
+        <v>0.9939120451665983</v>
       </c>
       <c r="H47">
-        <v>1.013175312539491</v>
+        <v>0.993435660773743</v>
       </c>
       <c r="I47">
-        <v>0.9931619337768488</v>
+        <v>0.9906469215535926</v>
       </c>
       <c r="J47">
-        <v>0.9579336841299908</v>
+        <v>0.9959513031813313</v>
       </c>
       <c r="K47">
-        <v>1.016223885421911</v>
+        <v>0.9908615863341106</v>
       </c>
       <c r="L47">
-        <v>0.9851113216013381</v>
+        <v>0.9904813140095031</v>
       </c>
       <c r="M47">
-        <v>1.070755083423398</v>
+        <v>0.9939061735181346</v>
       </c>
       <c r="N47">
-        <v>1.070764926170405</v>
+        <v>0.9939120451665983</v>
       </c>
       <c r="O47">
-        <v>0.9852273776487803</v>
+        <v>0.9972756153169642</v>
       </c>
       <c r="P47">
-        <v>0.9731623716785669</v>
+        <v>0.9967002157250392</v>
       </c>
       <c r="Q47">
-        <v>1.013739893822655</v>
+        <v>0.9961544252668423</v>
       </c>
       <c r="R47">
-        <v>0.9865000186322082</v>
+        <v>0.9956120307412738</v>
       </c>
       <c r="S47">
-        <v>1.013739893822655</v>
+        <v>0.9961544252668423</v>
       </c>
       <c r="T47">
-        <v>1.007566245516757</v>
+        <v>0.9951870343476049</v>
       </c>
       <c r="U47">
-        <v>1.020205981647487</v>
+        <v>0.9949320365114035</v>
       </c>
       <c r="V47">
-        <v>0.9978369758746397</v>
+        <v>0.9935861578086196</v>
       </c>
     </row>
     <row r="48" spans="1:22">
@@ -3779,63 +3782,131 @@
         <v>46</v>
       </c>
       <c r="C48">
+        <v>1.070764926170405</v>
+      </c>
+      <c r="D48">
+        <v>1.013175312539491</v>
+      </c>
+      <c r="E48">
+        <v>0.9572794427580701</v>
+      </c>
+      <c r="F48">
+        <v>0.9890453005990636</v>
+      </c>
+      <c r="G48">
+        <v>1.070764926170405</v>
+      </c>
+      <c r="H48">
+        <v>1.013175312539491</v>
+      </c>
+      <c r="I48">
+        <v>0.9931619337768488</v>
+      </c>
+      <c r="J48">
+        <v>0.9579336841299908</v>
+      </c>
+      <c r="K48">
+        <v>1.016223885421911</v>
+      </c>
+      <c r="L48">
+        <v>0.9851113216013381</v>
+      </c>
+      <c r="M48">
+        <v>1.070755083423398</v>
+      </c>
+      <c r="N48">
+        <v>1.070764926170405</v>
+      </c>
+      <c r="O48">
+        <v>0.9852273776487803</v>
+      </c>
+      <c r="P48">
+        <v>0.9731623716785669</v>
+      </c>
+      <c r="Q48">
+        <v>1.013739893822655</v>
+      </c>
+      <c r="R48">
+        <v>0.9865000186322082</v>
+      </c>
+      <c r="S48">
+        <v>1.013739893822655</v>
+      </c>
+      <c r="T48">
+        <v>1.007566245516757</v>
+      </c>
+      <c r="U48">
+        <v>1.020205981647487</v>
+      </c>
+      <c r="V48">
+        <v>0.9978369758746397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49">
         <v>1.135887431332871</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>1.095870211077832</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <v>0.8794992804952897</v>
       </c>
-      <c r="F48">
+      <c r="F49">
         <v>1.003917927306676</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>1.135887431332871</v>
       </c>
-      <c r="H48">
+      <c r="H49">
         <v>1.095870211077832</v>
       </c>
-      <c r="I48">
+      <c r="I49">
         <v>0.9577438896043622</v>
       </c>
-      <c r="J48">
+      <c r="J49">
         <v>0.929432008269752</v>
       </c>
-      <c r="K48">
+      <c r="K49">
         <v>1.035143566543755</v>
       </c>
-      <c r="L48">
+      <c r="L49">
         <v>1.024319544542498</v>
       </c>
-      <c r="M48">
+      <c r="M49">
         <v>1.135791712345791</v>
       </c>
-      <c r="N48">
+      <c r="N49">
         <v>1.135887431332871</v>
       </c>
-      <c r="O48">
+      <c r="O49">
         <v>0.987684745786561</v>
       </c>
-      <c r="P48">
+      <c r="P49">
         <v>0.9417086039009828</v>
       </c>
-      <c r="Q48">
+      <c r="Q49">
         <v>1.037085640968664</v>
       </c>
-      <c r="R48">
+      <c r="R49">
         <v>0.9930958062932659</v>
       </c>
-      <c r="S48">
+      <c r="S49">
         <v>1.037085640968664</v>
       </c>
-      <c r="T48">
+      <c r="T49">
         <v>1.028793712553167</v>
       </c>
-      <c r="U48">
+      <c r="U49">
         <v>1.050212456309108</v>
       </c>
-      <c r="V48">
+      <c r="V49">
         <v>1.007726732396629</v>
       </c>
     </row>

</xml_diff>